<commit_message>
Fix doc. InvalidateKey is not encrypted
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin_g\Documents\_PRIVATE\Arduino\EnigmaIOT\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin_g\Documents\_PRIVATE\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1101,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1339,7 +1339,7 @@
       <c r="H22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate and process indicate message
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin_g\Documents\_PRIVATE\Arduino\libraries\EnigmaIOT\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE432E27-1D4F-4784-AF20-9C9E0EE25423}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>FF</t>
   </si>
@@ -261,12 +262,15 @@
   </si>
   <si>
     <t>OTA update payload</t>
+  </si>
+  <si>
+    <t>Indicate (identify node)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1029,7 +1033,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="Rohde &amp; Schwarz Coloured PrivotTable">
-    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10">
+    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -1041,7 +1045,7 @@
       <tableStyleElement type="pageFieldLabels" dxfId="7"/>
       <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6">
+    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="totalRow" dxfId="3"/>
@@ -1311,11 +1315,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:U74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:U76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1738,109 +1742,110 @@
         <v>2</v>
       </c>
     </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F53" s="1"/>
+      <c r="H53" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H54" t="s">
+      <c r="F54" s="1"/>
+      <c r="G54" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G55" s="10" t="s">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G57" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H55" s="20" t="s">
+      <c r="H57" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="I55" s="22" t="s">
+      <c r="I57" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="J55" s="24"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="23"/>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E57" s="13" t="s">
+      <c r="J57" s="24"/>
+      <c r="K57" s="24"/>
+      <c r="L57" s="23"/>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E59" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D58" s="10" t="s">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D60" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E60" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F58" s="28"/>
-      <c r="G58" s="29" t="s">
+      <c r="F60" s="28"/>
+      <c r="G60" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="H58" s="30"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="29" t="s">
+      <c r="H60" s="30"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="K58" s="30"/>
-      <c r="L58" s="29" t="s">
+      <c r="K60" s="30"/>
+      <c r="L60" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="M58" s="30"/>
-      <c r="N58" s="31"/>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C60" s="14" t="s">
+      <c r="M60" s="30"/>
+      <c r="N60" s="31"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C62" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="21" t="s">
+      <c r="D62" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E60" s="25" t="s">
+      <c r="E62" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F62" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D62" s="10" t="s">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D64" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="27" t="s">
+      <c r="E64" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F62" s="28"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="30" t="s">
+      <c r="F64" s="28"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="J62" s="30"/>
-      <c r="K62" s="30"/>
-      <c r="L62" s="30"/>
-      <c r="M62" s="30"/>
-      <c r="N62" s="31"/>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D64" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E64" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F64" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="J64" s="30"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="30"/>
+      <c r="M64" s="30"/>
+      <c r="N64" s="31"/>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D66" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>2</v>
@@ -1848,13 +1853,13 @@
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D68" s="14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E68" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>2</v>
@@ -1862,13 +1867,13 @@
     </row>
     <row r="70" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D70" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E70" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F70" s="26" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>2</v>
@@ -1876,13 +1881,13 @@
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D72" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E72" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F72" s="25" t="s">
-        <v>70</v>
+      <c r="F72" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>2</v>
@@ -1890,15 +1895,29 @@
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D74" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E74" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D76" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G76" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1910,13 +1929,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B12:B14 B19:B20 I61 I63 H18 H42:H51 F64:F74 E60" numberStoredAsText="1"/>
+    <ignoredError sqref="B12:B14 B19:B20 I63 I65 H18 H42:H51 F66:F76 E62 H54" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1928,7 +1947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Start migration to ChaCha+Poly1305
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE432E27-1D4F-4784-AF20-9C9E0EE25423}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C050CE9-BF12-461B-86FF-6A7770FA0483}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>FF</t>
   </si>
@@ -48,9 +48,6 @@
     <t>NodeID (2 byte)</t>
   </si>
   <si>
-    <t>CRC (4 byte)</t>
-  </si>
-  <si>
     <t>&lt;------------------------------------</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>01</t>
   </si>
   <si>
-    <t>Sensor Data (n)</t>
-  </si>
-  <si>
     <t>Invalidate key</t>
   </si>
   <si>
@@ -108,15 +102,6 @@
     <t>Random (4 byte)</t>
   </si>
   <si>
-    <t>IV (16 byte)</t>
-  </si>
-  <si>
-    <t>Random 16 Byte</t>
-  </si>
-  <si>
-    <t>IV 16 Byte</t>
-  </si>
-  <si>
     <t>CRC is generated before encryption and checked after decryption</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>Sensor Command</t>
   </si>
   <si>
-    <t>Payload (n)</t>
-  </si>
-  <si>
     <t>02</t>
   </si>
   <si>
@@ -255,9 +237,6 @@
     <t>Payload (up to 224 bytes)</t>
   </si>
   <si>
-    <t>Payload (up to 225 bytes)</t>
-  </si>
-  <si>
     <t>CONTROL COMMANDS PAYLOAD</t>
   </si>
   <si>
@@ -265,6 +244,27 @@
   </si>
   <si>
     <t>Indicate (identify node)</t>
+  </si>
+  <si>
+    <t>Tag (16 byte)</t>
+  </si>
+  <si>
+    <t>IV 12 Byte</t>
+  </si>
+  <si>
+    <t>Sensor Data (up to 215 bytes)</t>
+  </si>
+  <si>
+    <t>Payload (up to 217 bytes)</t>
+  </si>
+  <si>
+    <t>Random 12 Byte</t>
+  </si>
+  <si>
+    <t>Tag is calculated using Poly1305 from last 8 bytes of Network Key</t>
+  </si>
+  <si>
+    <t>Tag is calculated using Poly1305 from last 8 bytes of Session Key + MsgID</t>
   </si>
 </sst>
 </file>
@@ -1318,20 +1318,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1341,14 +1341,14 @@
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C4" s="32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
       <c r="J4" s="32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K4" s="32"/>
       <c r="L4" s="32"/>
@@ -1366,19 +1366,22 @@
         <v>0</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1387,19 +1390,19 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
@@ -1407,116 +1410,127 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="J9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>8</v>
+        <v>74</v>
+      </c>
+      <c r="M9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="G14" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C13" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="8" t="s">
+      <c r="H14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>8</v>
+      <c r="L14" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="I17" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G18" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>7</v>
@@ -1526,25 +1540,24 @@
       </c>
       <c r="M18" s="8"/>
       <c r="N18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18" s="8"/>
+        <v>74</v>
+      </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>7</v>
@@ -1554,7 +1567,7 @@
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="1" t="s">
@@ -1563,10 +1576,10 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="R23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S23">
         <v>6</v>
@@ -1580,97 +1593,97 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="S24" t="s">
+        <v>19</v>
+      </c>
+      <c r="T24" t="s">
+        <v>20</v>
+      </c>
+      <c r="U24" t="s">
         <v>21</v>
-      </c>
-      <c r="T24" t="s">
-        <v>22</v>
-      </c>
-      <c r="U24" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="I28" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="F29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="I31" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C33" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C34" s="12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C36" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C39" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H42" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G43" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I43" s="16"/>
     </row>
@@ -1679,7 +1692,7 @@
         <v>81</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D44" s="24"/>
       <c r="E44" s="23"/>
@@ -1690,15 +1703,15 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="H46" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="G47" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
@@ -1706,7 +1719,7 @@
         <v>82</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D48" s="23"/>
       <c r="F48" s="1" t="s">
@@ -1715,18 +1728,18 @@
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H50" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G51" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H51" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I51" s="22" t="s">
         <v>48</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>54</v>
       </c>
       <c r="J51" s="23"/>
     </row>
@@ -1735,7 +1748,7 @@
         <v>82</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D52" s="23"/>
       <c r="F52" s="1" t="s">
@@ -1745,32 +1758,32 @@
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F53" s="1"/>
       <c r="H53" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F54" s="1"/>
       <c r="G54" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H56" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G57" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H57" s="20" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="J57" s="24"/>
       <c r="K57" s="24"/>
@@ -1778,41 +1791,41 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E59" s="13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D60" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F60" s="28"/>
       <c r="G60" s="29" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H60" s="30"/>
       <c r="I60" s="29"/>
       <c r="J60" s="29" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="K60" s="30"/>
       <c r="L60" s="29" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="M60" s="30"/>
       <c r="N60" s="31"/>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C62" s="14" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D62" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E62" s="25" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>2</v>
@@ -1820,16 +1833,16 @@
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D64" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" s="27" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F64" s="28"/>
       <c r="G64" s="29"/>
       <c r="H64" s="30"/>
       <c r="I64" s="30" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J64" s="30"/>
       <c r="K64" s="30"/>
@@ -1839,13 +1852,13 @@
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D66" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E66" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F66" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>2</v>
@@ -1853,13 +1866,13 @@
     </row>
     <row r="68" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D68" s="14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E68" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>2</v>
@@ -1867,13 +1880,13 @@
     </row>
     <row r="70" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D70" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E70" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F70" s="26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>2</v>
@@ -1881,13 +1894,13 @@
     </row>
     <row r="72" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D72" s="14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E72" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="26" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>2</v>
@@ -1895,13 +1908,13 @@
     </row>
     <row r="74" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D74" s="14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E74" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="25" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>2</v>
@@ -1909,13 +1922,13 @@
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D76" s="14" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E76" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>2</v>
@@ -1929,7 +1942,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B12:B14 B19:B20 I63 I65 H18 H42:H51 F66:F76 E62 H54" numberStoredAsText="1"/>
+    <ignoredError sqref="B12 B19:B20 I63 I65 H18 H42:H51 F66:F76 E62 H54 H14" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve OTA update resiliency
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -16,12 +16,13 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
   <si>
     <t>FF</t>
   </si>
@@ -264,6 +265,9 @@
   </si>
   <si>
     <t>Kgw (32 byte)</t>
+  </si>
+  <si>
+    <t>Last good msg index (16 bit int)</t>
   </si>
 </sst>
 </file>
@@ -702,7 +706,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -739,6 +743,9 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1338,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:U86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1361,21 +1368,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="J4" s="33" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="J4" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1404,10 +1411,10 @@
       <c r="F6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="40"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1446,10 +1453,10 @@
       <c r="L8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="N8" s="39"/>
+      <c r="N8" s="40"/>
       <c r="O8" t="s">
         <v>68</v>
       </c>
@@ -1491,11 +1498,11 @@
       <c r="F13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
       <c r="J13" s="7" t="s">
         <v>65</v>
       </c>
@@ -1597,10 +1604,10 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="D23" s="38"/>
+      <c r="D23" s="39"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
@@ -1609,34 +1616,43 @@
       <c r="C24" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="36"/>
+      <c r="E24" s="37"/>
       <c r="F24" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="I24" s="38" t="s">
+      <c r="G24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I25" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="J24" s="38"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="H25" s="9" t="s">
+      <c r="J25" s="39"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I26" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="J25" s="34" t="s">
+      <c r="J26" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="36"/>
-      <c r="L25" s="34" t="s">
+      <c r="K26" s="37"/>
+      <c r="L26" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="M25" s="36"/>
-      <c r="N25" s="32" t="s">
+      <c r="M26" s="36"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="33" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1960,7 +1976,12 @@
       <c r="F77" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="G77" s="1" t="s">
+      <c r="G77" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="H77" s="26"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1993,10 +2014,10 @@
       </c>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="N85" s="37" t="s">
+      <c r="N85" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O85" s="37"/>
+      <c r="O85" s="38"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B86" s="21">
@@ -2009,18 +2030,18 @@
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="N85:O85"/>
-    <mergeCell ref="J25:K25"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="I25:J25"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="M8:N8"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B20:B21 I68 I70 H19 H47:H56 F71:F81 E67 H59 H15 B24 H25" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B20:B21 I68 I70 H19 H47:H56 F71:F81 E67 H59 H15 B24" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add option to request and report node RSSI
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin_g\Documents\_PRIVATE\Arduino\libraries\EnigmaIOT\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BBFBD-5E30-456D-B0E5-254BA75520B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7410" yWindow="1020" windowWidth="30255" windowHeight="16530"/>
+    <workbookView xWindow="7755" yWindow="1365" windowWidth="30255" windowHeight="16530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
   <si>
     <t>FF</t>
   </si>
@@ -240,9 +240,6 @@
     <t>OTA binary data (Up to 212 bytes)</t>
   </si>
   <si>
-    <t>Transmit time (32 bits integer)</t>
-  </si>
-  <si>
     <t>Clock request</t>
   </si>
   <si>
@@ -268,12 +265,30 @@
   </si>
   <si>
     <t>Last good msg index (16 bit int)</t>
+  </si>
+  <si>
+    <t>RSSI (1 byte)</t>
+  </si>
+  <si>
+    <t>Measure RSSI</t>
+  </si>
+  <si>
+    <t>Report RSSI</t>
+  </si>
+  <si>
+    <t>Channel (1 byte)</t>
+  </si>
+  <si>
+    <t>Reset configuration</t>
+  </si>
+  <si>
+    <t>Reset confirm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -706,7 +721,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -759,9 +774,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1060,7 +1072,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="Rohde &amp; Schwarz Coloured PrivotTable">
-    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10">
+    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -1072,7 +1084,7 @@
       <tableStyleElement type="pageFieldLabels" dxfId="7"/>
       <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6">
+    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="totalRow" dxfId="3"/>
@@ -1342,11 +1354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:U86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>29</v>
@@ -1411,10 +1423,10 @@
       <c r="F6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="39"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1445,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1445,7 +1457,7 @@
         <v>70</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
@@ -1453,10 +1465,10 @@
       <c r="L8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="N8" s="40"/>
+      <c r="N8" s="39"/>
       <c r="O8" t="s">
         <v>68</v>
       </c>
@@ -1604,10 +1616,10 @@
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C23" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="39"/>
+      <c r="C23" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="38"/>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" s="9" t="s">
@@ -1617,7 +1629,7 @@
         <v>70</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E24" s="37"/>
       <c r="F24" s="32" t="s">
@@ -1628,10 +1640,10 @@
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I25" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="39"/>
+      <c r="I25" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G26" s="10" t="s">
@@ -1644,11 +1656,11 @@
         <v>70</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K26" s="37"/>
       <c r="L26" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M26" s="36"/>
       <c r="N26" s="37"/>
@@ -1977,7 +1989,7 @@
         <v>32</v>
       </c>
       <c r="G77" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H77" s="26"/>
       <c r="I77" s="26"/>
@@ -1999,7 +2011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D81" s="14" t="s">
         <v>54</v>
       </c>
@@ -2013,23 +2025,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="N85" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="O85" s="38"/>
-    </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B86" s="21">
-        <v>5</v>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="G84" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="21">
+        <v>85</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>83</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B89" s="21">
+        <v>86</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="N85:O85"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="I25:J25"/>
     <mergeCell ref="D24:E24"/>
@@ -2041,13 +2095,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B20:B21 I68 I70 H19 H47:H56 F71:F81 E67 H59 H15 B24" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B20:B21 I68 I70 H19 H47:H56 F71:F81 E67 H59 H15 B24 H88 H84" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2059,7 +2113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
New unencrypted message from node
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\martin_g\Documents\_PRIVATE\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4BBFBD-5E30-456D-B0E5-254BA75520B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="1365" windowWidth="30255" windowHeight="16530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7755" yWindow="1365" windowWidth="30255" windowHeight="16530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="90">
   <si>
     <t>FF</t>
   </si>
@@ -45,9 +44,6 @@
     <t>&lt;------------------------------------</t>
   </si>
   <si>
-    <t>Sensor Data</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -96,18 +92,12 @@
     <t>This is answered in case a node trying to send a message is not registered or key is wrong</t>
   </si>
   <si>
-    <t>Sensor</t>
-  </si>
-  <si>
     <t>Gateway</t>
   </si>
   <si>
     <t>Counter (2 byte)</t>
   </si>
   <si>
-    <t>Sensor Command</t>
-  </si>
-  <si>
     <t>02</t>
   </si>
   <si>
@@ -283,12 +273,30 @@
   </si>
   <si>
     <t>Reset confirm</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Node Data</t>
+  </si>
+  <si>
+    <t>Node Command</t>
+  </si>
+  <si>
+    <t>Node Data (unencrypted)</t>
+  </si>
+  <si>
+    <t>Payload Type (1 byte)</t>
+  </si>
+  <si>
+    <t>Sensor Data (up to 244 bytes)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -721,7 +729,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -780,6 +788,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1072,7 +1089,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="Rohde &amp; Schwarz Coloured PrivotTable">
-    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -1084,7 +1101,7 @@
       <tableStyleElement type="pageFieldLabels" dxfId="7"/>
       <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="totalRow" dxfId="3"/>
@@ -1354,19 +1371,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U89"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" customWidth="1"/>
@@ -1381,14 +1398,14 @@
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
       <c r="C4" s="34" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="J4" s="34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K4" s="34"/>
       <c r="L4" s="34"/>
@@ -1412,19 +1429,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H6" s="39"/>
       <c r="I6" s="1" t="s">
@@ -1433,7 +1450,7 @@
       <c r="J6" s="10"/>
       <c r="L6" s="10"/>
       <c r="O6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1445,7 +1462,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1454,23 +1471,23 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M8" s="39" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N8" s="39"/>
       <c r="O8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -1491,43 +1508,43 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H13" s="36"/>
       <c r="I13" s="37"/>
       <c r="J13" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -1535,573 +1552,602 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="9">
+        <v>11</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="N20" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G19" s="10" t="s">
+      <c r="C22" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C24" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="38"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="37"/>
+      <c r="F25" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I26" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="38"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="8" t="s">
+      <c r="H27" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="M19" s="8"/>
-      <c r="N19" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="7"/>
-      <c r="J21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C23" s="38" t="s">
+      <c r="J27" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="38"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I25" s="38" t="s">
+      <c r="K27" s="37"/>
+      <c r="L27" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G26" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="M26" s="36"/>
-      <c r="N26" s="37"/>
-      <c r="O26" s="33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-      <c r="R28" t="s">
-        <v>14</v>
-      </c>
-      <c r="S28">
-        <v>6</v>
-      </c>
-      <c r="T28">
-        <v>2</v>
-      </c>
-      <c r="U28">
-        <v>32</v>
+      <c r="M27" s="36"/>
+      <c r="N27" s="37"/>
+      <c r="O27" s="33" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="S29" t="s">
+      <c r="R29" t="s">
+        <v>13</v>
+      </c>
+      <c r="S29">
+        <v>6</v>
+      </c>
+      <c r="T29">
+        <v>2</v>
+      </c>
+      <c r="U29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="S30" t="s">
+        <v>14</v>
+      </c>
+      <c r="T30" t="s">
         <v>15</v>
       </c>
-      <c r="T29" t="s">
+      <c r="U30" t="s">
         <v>16</v>
       </c>
-      <c r="U29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="I34" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="F34" s="1" t="s">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C40" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C42" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="H48" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G49" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="I36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="4" t="s">
+      <c r="H49" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="16"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B50" s="21">
+        <v>81</v>
+      </c>
+      <c r="C50" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H50" s="17"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G53" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B54" s="20">
+        <v>82</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C41" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C44" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="H47" s="15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="G48" s="10" t="s">
+      <c r="D54" s="23"/>
+      <c r="F54" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G57" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I48" s="16"/>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B49" s="21">
-        <v>81</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="1" t="s">
+      <c r="H57" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I57" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J57" s="23"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B58" s="20">
+        <v>82</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="F58" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="H51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G52" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H52" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B53" s="20">
-        <v>82</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D53" s="23"/>
-      <c r="F53" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="H55" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G56" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I56" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="J56" s="23"/>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B57" s="20">
-        <v>82</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="23"/>
-      <c r="F57" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="F58" s="1"/>
-      <c r="H58" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F59" s="1"/>
-      <c r="G59" s="10" t="s">
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="F60" s="1"/>
+      <c r="G60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H59" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="H61" t="s">
+      <c r="H60" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G63" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I63" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J63" s="24"/>
+      <c r="K63" s="24"/>
+      <c r="L63" s="23"/>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="E65" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G62" s="10" t="s">
+    <row r="66" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D66" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H62" s="20" t="s">
+      <c r="E66" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" s="28"/>
+      <c r="G66" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H66" s="30"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K66" s="30"/>
+      <c r="L66" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="I62" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="J62" s="24"/>
-      <c r="K62" s="24"/>
-      <c r="L62" s="23"/>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="E64" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D65" s="10" t="s">
+      <c r="M66" s="30"/>
+      <c r="N66" s="31"/>
+    </row>
+    <row r="68" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C68" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D70" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="27" t="s">
+      <c r="E70" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" s="28"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="J70" s="30"/>
+      <c r="K70" s="31"/>
+    </row>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D72" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F72" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D74" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D76" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F65" s="28"/>
-      <c r="G65" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="H65" s="30"/>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="K65" s="30"/>
-      <c r="L65" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="M65" s="30"/>
-      <c r="N65" s="31"/>
-    </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C67" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="21" t="s">
+      <c r="E76" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E67" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="F67" s="1" t="s">
+      <c r="F76" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D69" s="10" t="s">
+    <row r="78" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D78" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G78" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H78" s="26"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D80" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D82" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" t="s">
+        <v>83</v>
+      </c>
+      <c r="G85" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F69" s="28"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="30"/>
-      <c r="I69" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="J69" s="30"/>
-      <c r="K69" s="31"/>
-    </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D71" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G71" s="1" t="s">
+      <c r="H85" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="21">
+        <v>85</v>
+      </c>
+      <c r="F86" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D73" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F73" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="G73" s="1" t="s">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>80</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B90" s="21">
+        <v>86</v>
+      </c>
+      <c r="C90" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D90" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F90" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D75" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F75" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D77" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E77" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F77" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="H77" s="26"/>
-      <c r="I77" s="26"/>
-      <c r="J77" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D79" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E79" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F79" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D81" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E81" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F81" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H83" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" t="s">
-        <v>86</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H84" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="21">
-        <v>85</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H87" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" t="s">
-        <v>83</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H88" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="21">
-        <v>86</v>
-      </c>
-      <c r="C89" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="G13:I13"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:N26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B20:B21 I68 I70 H19 H47:H56 F71:F81 E67 H59 H15 B24 H88 H84" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I69 I71 H20 H48:H57 F72:F82 E68 H60 H15 B25 H89 H85" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2113,7 +2159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Implement Payload encoding type on Node
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t>FF</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Tag (16 byte)</t>
   </si>
   <si>
-    <t>Sensor Data (up to 215 bytes)</t>
-  </si>
-  <si>
     <t>Payload (up to 217 bytes)</t>
   </si>
   <si>
@@ -291,6 +288,12 @@
   </si>
   <si>
     <t>Sensor Data (up to 244 bytes)</t>
+  </si>
+  <si>
+    <t>Sensor Data (up to 214 bytes)</t>
+  </si>
+  <si>
+    <t>Payload (up to 216 bytes)</t>
   </si>
 </sst>
 </file>
@@ -729,7 +732,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -772,22 +775,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -799,6 +793,21 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1374,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1385,33 +1394,33 @@
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="3.42578125" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="J4" s="34" t="s">
+      <c r="C4" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="J4" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1429,10 +1438,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>26</v>
@@ -1440,17 +1449,17 @@
       <c r="F6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="10"/>
       <c r="L6" s="10"/>
       <c r="O6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1462,7 +1471,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1471,10 +1480,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
@@ -1482,12 +1491,12 @@
       <c r="L8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="39" t="s">
+      <c r="M8" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="39"/>
+      <c r="N8" s="42"/>
       <c r="O8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -1508,7 +1517,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -1516,7 +1525,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>17</v>
@@ -1527,24 +1536,27 @@
       <c r="F13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="7" t="s">
+      <c r="G13" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="45"/>
+      <c r="I13" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="44"/>
+      <c r="K13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -1555,7 +1567,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>17</v>
@@ -1563,17 +1575,20 @@
       <c r="K15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="7" t="s">
+      <c r="L15" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="7" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2"/>
     </row>
@@ -1588,13 +1603,13 @@
         <v>24</v>
       </c>
       <c r="E17" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" s="41"/>
-      <c r="H17" s="42"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1613,7 +1628,7 @@
         <v>29</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>17</v>
@@ -1621,11 +1636,14 @@
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="7" t="s">
+      <c r="L20" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="8"/>
+      <c r="O20" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1640,7 +1658,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>17</v>
@@ -1649,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="7" t="s">
@@ -1661,22 +1679,22 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C24" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="38"/>
+      <c r="C24" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="E25" s="37"/>
+        <v>66</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="35"/>
       <c r="F25" s="32" t="s">
         <v>62</v>
       </c>
@@ -1685,10 +1703,10 @@
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I26" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" s="38"/>
+      <c r="I26" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" s="41"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1698,17 +1716,17 @@
         <v>53</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J27" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="K27" s="35"/>
+      <c r="L27" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="37"/>
-      <c r="L27" s="35" t="s">
-        <v>73</v>
-      </c>
       <c r="M27" s="36"/>
-      <c r="N27" s="37"/>
+      <c r="N27" s="35"/>
       <c r="O27" s="33" t="s">
         <v>62</v>
       </c>
@@ -1976,7 +1994,7 @@
       <c r="G70" s="29"/>
       <c r="H70" s="30"/>
       <c r="I70" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J70" s="30"/>
       <c r="K70" s="31"/>
@@ -2034,7 +2052,7 @@
         <v>29</v>
       </c>
       <c r="G78" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H78" s="26"/>
       <c r="I78" s="26"/>
@@ -2072,12 +2090,12 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>6</v>
@@ -2096,12 +2114,12 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>6</v>
@@ -2115,10 +2133,10 @@
         <v>86</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>2</v>
@@ -2131,12 +2149,12 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
-    <mergeCell ref="G13:I13"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement Payload encoding type on Gateway
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>FF</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Reason (1 byte)</t>
   </si>
   <si>
-    <t>If sensor is not registered gateway ignores it</t>
-  </si>
-  <si>
     <t>Key is invalidated periodically (ex. Each day)</t>
   </si>
   <si>
@@ -287,13 +284,25 @@
     <t>Payload Type (1 byte)</t>
   </si>
   <si>
-    <t>Sensor Data (up to 244 bytes)</t>
-  </si>
-  <si>
-    <t>Sensor Data (up to 214 bytes)</t>
-  </si>
-  <si>
     <t>Payload (up to 216 bytes)</t>
+  </si>
+  <si>
+    <t>Encoding Id (1 byte)</t>
+  </si>
+  <si>
+    <t>If node is not registered gateway ignores it</t>
+  </si>
+  <si>
+    <t>Node Data (up to 244 bytes)</t>
+  </si>
+  <si>
+    <t>Node Data (up to 214 bytes)</t>
+  </si>
+  <si>
+    <t>02/03</t>
+  </si>
+  <si>
+    <t>02 = SET command, 03 = GET command</t>
   </si>
 </sst>
 </file>
@@ -775,6 +784,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -802,12 +814,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -1383,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1394,33 +1403,33 @@
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="J4" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
+      <c r="C4" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="J4" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1438,28 +1447,28 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="42"/>
+      <c r="G6" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="45"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="10"/>
       <c r="L6" s="10"/>
       <c r="O6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -1471,7 +1480,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1480,23 +1489,23 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="42"/>
+        <v>17</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" s="45"/>
       <c r="O8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -1517,7 +1526,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -1525,38 +1534,38 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="H13" s="45"/>
-      <c r="I13" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" s="44"/>
+        <v>23</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="I13" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="35"/>
       <c r="K13" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -1564,33 +1573,36 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="46" t="s">
+      <c r="L15" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>87</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>90</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2"/>
+      <c r="I16" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
@@ -1600,23 +1612,23 @@
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
+        <v>86</v>
+      </c>
+      <c r="F17" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="41"/>
+      <c r="H17" s="42"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="I19" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J19" s="2"/>
     </row>
@@ -1625,53 +1637,50 @@
         <v>6</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
       <c r="L20" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="M20" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="N20" s="8"/>
-      <c r="O20" s="7" t="s">
         <v>62</v>
+      </c>
+      <c r="M20" s="46"/>
+      <c r="N20" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="1" t="s">
@@ -1679,64 +1688,64 @@
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C24" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="44"/>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="35"/>
+        <v>65</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="38"/>
       <c r="F25" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I26" s="41" t="s">
-        <v>69</v>
-      </c>
-      <c r="J26" s="41"/>
+      <c r="I26" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" s="44"/>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J27" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" s="38"/>
+      <c r="L27" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="35"/>
-      <c r="L27" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="M27" s="36"/>
-      <c r="N27" s="35"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="38"/>
       <c r="O27" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="R29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S29">
         <v>6</v>
@@ -1750,21 +1759,21 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S30" t="s">
+        <v>13</v>
+      </c>
+      <c r="T30" t="s">
         <v>14</v>
       </c>
-      <c r="T30" t="s">
+      <c r="U30" t="s">
         <v>15</v>
-      </c>
-      <c r="U30" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.2">
@@ -1785,49 +1794,49 @@
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C40" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D40" s="12"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C41" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C42" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="45" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C45" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.2">
       <c r="H48" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
@@ -1844,7 +1853,7 @@
         <v>81</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="23"/>
@@ -1855,7 +1864,7 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
@@ -1863,7 +1872,7 @@
         <v>6</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
@@ -1871,7 +1880,7 @@
         <v>82</v>
       </c>
       <c r="C54" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D54" s="23"/>
       <c r="F54" s="1" t="s">
@@ -1880,7 +1889,7 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
@@ -1888,10 +1897,10 @@
         <v>6</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J57" s="23"/>
     </row>
@@ -1900,7 +1909,7 @@
         <v>82</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58" s="23"/>
       <c r="F58" s="1" t="s">
@@ -1910,7 +1919,7 @@
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
       <c r="F59" s="1"/>
       <c r="H59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
@@ -1919,12 +1928,12 @@
         <v>6</v>
       </c>
       <c r="H60" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
@@ -1932,10 +1941,10 @@
         <v>6</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J63" s="24"/>
       <c r="K63" s="24"/>
@@ -1943,7 +1952,7 @@
     </row>
     <row r="65" spans="3:14" x14ac:dyDescent="0.2">
       <c r="E65" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="3:14" x14ac:dyDescent="0.2">
@@ -1951,33 +1960,33 @@
         <v>6</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F66" s="28"/>
       <c r="G66" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H66" s="30"/>
       <c r="I66" s="29"/>
       <c r="J66" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K66" s="30"/>
       <c r="L66" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M66" s="30"/>
       <c r="N66" s="31"/>
     </row>
     <row r="68" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C68" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D68" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>2</v>
@@ -1988,20 +1997,20 @@
         <v>6</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F70" s="28"/>
       <c r="G70" s="29"/>
       <c r="H70" s="30"/>
       <c r="I70" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J70" s="30"/>
       <c r="K70" s="31"/>
     </row>
     <row r="72" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D72" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E72" s="20" t="s">
         <v>0</v>
@@ -2015,13 +2024,13 @@
     </row>
     <row r="74" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D74" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E74" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>2</v>
@@ -2029,13 +2038,13 @@
     </row>
     <row r="76" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D76" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E76" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F76" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>2</v>
@@ -2043,16 +2052,16 @@
     </row>
     <row r="78" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D78" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E78" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F78" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G78" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H78" s="26"/>
       <c r="I78" s="26"/>
@@ -2062,13 +2071,13 @@
     </row>
     <row r="80" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D80" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E80" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F80" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>2</v>
@@ -2076,13 +2085,13 @@
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D82" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E82" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>2</v>
@@ -2090,18 +2099,18 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G85" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
@@ -2114,18 +2123,18 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H89" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
@@ -2133,17 +2142,17 @@
         <v>86</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D90" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="L27:N27"/>
     <mergeCell ref="F17:H17"/>
@@ -2155,11 +2164,12 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="G13:H13"/>
+    <mergeCell ref="L20:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I69 I71 H20 H48:H57 F72:F82 E68 H60 H15 B25 H89 H85" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I69 I71 H20 H48:H57 F72:F82 E68 H60 B25 H89 H85" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add set node name control message codes
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\martin_g\Documents\_PRIVATE\Arduino\libraries\EnigmaIOT\img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC6F70-2623-4438-AB6C-9EAF6819DDA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7755" yWindow="1365" windowWidth="30255" windowHeight="16530"/>
+    <workbookView xWindow="9360" yWindow="2430" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="99">
   <si>
     <t>FF</t>
   </si>
@@ -300,12 +301,30 @@
   </si>
   <si>
     <t>02 = SET command, 03 = GET command</t>
+  </si>
+  <si>
+    <t>Node Name (up to 32 bytes)</t>
+  </si>
+  <si>
+    <t>Set Node Name</t>
+  </si>
+  <si>
+    <t>Set node name result</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Result code (1 byte)</t>
+  </si>
+  <si>
+    <t>0: OK,  -1: Already used,  -2: Too long</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -738,7 +757,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -812,6 +831,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1104,7 +1129,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="Rohde &amp; Schwarz Coloured PrivotTable">
-    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10">
+    <tableStyle name="Rohde &amp; Schwarz Coloured PrivotTable" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="15"/>
       <tableStyleElement type="headerRow" dxfId="14"/>
       <tableStyleElement type="totalRow" dxfId="13"/>
@@ -1116,7 +1141,7 @@
       <tableStyleElement type="pageFieldLabels" dxfId="7"/>
       <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
-    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6">
+    <tableStyle name="Rohde &amp; Schwarz Coloured Table" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="wholeTable" dxfId="5"/>
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="totalRow" dxfId="3"/>
@@ -1386,11 +1411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:U90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B4:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I99" sqref="I99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2080,7 +2105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D82" s="14" t="s">
         <v>50</v>
       </c>
@@ -2094,12 +2119,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>81</v>
       </c>
@@ -2110,7 +2135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B86" s="21">
         <v>85</v>
       </c>
@@ -2118,12 +2143,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>78</v>
       </c>
@@ -2134,7 +2159,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B90" s="21">
         <v>86</v>
       </c>
@@ -2148,8 +2173,49 @@
         <v>2</v>
       </c>
     </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B94" s="21">
+        <v>87</v>
+      </c>
+      <c r="C94" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D94" s="47"/>
+      <c r="F94" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G96" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="I96" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="J96" s="47"/>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I97" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="I96:J96"/>
     <mergeCell ref="J27:K27"/>
     <mergeCell ref="L27:N27"/>
     <mergeCell ref="F17:H17"/>
@@ -2166,13 +2232,13 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I69 I71 H20 H48:H57 F72:F82 E68 H60 B25 H89 H85" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I69 I71 H20 H48:H57 F72:F82 E68 H60 B25 H89 H85 H96" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2184,7 +2250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Implement node name set and get through Output Gateway
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821E654E-C793-4D41-A197-A0535FA37A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A4CEA3-0BEB-4C8D-8781-B0BA2DE3F60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="2430" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="2610" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="107">
   <si>
     <t>FF</t>
   </si>
@@ -309,9 +309,6 @@
     <t>Result code (1 byte)</t>
   </si>
   <si>
-    <t>0: OK,  -1: Already used,  -2: Too long</t>
-  </si>
-  <si>
     <t>Node name (up to 32 bytes)</t>
   </si>
   <si>
@@ -322,6 +319,30 @@
   </si>
   <si>
     <t>17</t>
+  </si>
+  <si>
+    <t>Get name</t>
+  </si>
+  <si>
+    <t>Name (up to 32 byte)</t>
+  </si>
+  <si>
+    <t>Set name</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>* address length depends on physical platform. 6 bytes to esp-now</t>
+  </si>
+  <si>
+    <t>0: OK,  -1: Already used,  -2: Too long, -3: Empty name,  -4: Message error</t>
+  </si>
+  <si>
+    <t>Report name</t>
+  </si>
+  <si>
+    <t>Address (6 byte)*</t>
   </si>
 </sst>
 </file>
@@ -760,7 +781,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -809,10 +830,22 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -829,9 +862,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1412,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U94"/>
+  <dimension ref="B4:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1437,21 +1467,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="J4" s="44" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="J4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1480,10 +1510,10 @@
       <c r="F6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="46"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1522,10 +1552,10 @@
       <c r="L8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="46" t="s">
+      <c r="M8" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="46"/>
+      <c r="N8" s="49"/>
       <c r="O8" t="s">
         <v>63</v>
       </c>
@@ -1567,10 +1597,10 @@
       <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="47"/>
+      <c r="H13" s="50"/>
       <c r="I13" s="34" t="s">
         <v>90</v>
       </c>
@@ -1639,11 +1669,11 @@
       <c r="E17" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="41" t="s">
+      <c r="F17" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="43"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1670,10 +1700,10 @@
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="47" t="s">
+      <c r="L20" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="47"/>
+      <c r="M20" s="50"/>
       <c r="N20" s="7" t="s">
         <v>61</v>
       </c>
@@ -1710,10 +1740,10 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="45"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1722,10 +1752,10 @@
       <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="32" t="s">
         <v>61</v>
       </c>
@@ -1734,10 +1764,10 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="45"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1749,24 +1779,24 @@
       <c r="I27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J27" s="38" t="s">
+      <c r="J27" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="K27" s="39"/>
-      <c r="L27" s="38" t="s">
+      <c r="K27" s="40"/>
+      <c r="L27" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="40"/>
-      <c r="N27" s="39"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="40"/>
       <c r="O27" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C29" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="45"/>
+      <c r="C29" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1775,10 +1805,10 @@
       <c r="C30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="E30" s="39"/>
+      <c r="D30" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="40"/>
       <c r="F30" s="37" t="s">
         <v>61</v>
       </c>
@@ -1787,25 +1817,25 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I31" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" s="45"/>
+      <c r="I31" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J32" s="38" t="s">
+      <c r="J32" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="39"/>
+      <c r="K32" s="40"/>
       <c r="L32" s="37" t="s">
         <v>61</v>
       </c>
@@ -1815,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.2">
@@ -2224,8 +2254,62 @@
         <v>2</v>
       </c>
     </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G97" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G100" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I100" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="J100" s="43"/>
+      <c r="K100" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="L100" s="42"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B101" t="s">
+        <v>105</v>
+      </c>
+      <c r="I101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B102" s="21">
+        <v>87</v>
+      </c>
+      <c r="C102" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102" s="42"/>
+      <c r="F102" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2242,11 +2326,14 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="I100:J100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I73 I75 H20 H52:H61 F76:F86 E72 H64 B25 H93 H89 B30 H32" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I73 I75 H20 H52:H61 F76:F86 E72 H64 B25 H93 H89 B30 H32 H97 H100" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Clean more compiler warnings
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A4CEA3-0BEB-4C8D-8781-B0BA2DE3F60A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DEB916-5DF0-4AAD-BDE2-9A4C774CCD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="2610" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -830,6 +830,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -839,13 +842,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,13 +860,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1444,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,21 +1467,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="J4" s="48" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="J4" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1510,10 +1510,10 @@
       <c r="F6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="49"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1552,10 +1552,10 @@
       <c r="L8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="49"/>
+      <c r="N8" s="42"/>
       <c r="O8" t="s">
         <v>63</v>
       </c>
@@ -1597,10 +1597,10 @@
       <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="50"/>
+      <c r="H13" s="43"/>
       <c r="I13" s="34" t="s">
         <v>90</v>
       </c>
@@ -1700,10 +1700,10 @@
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="50" t="s">
+      <c r="L20" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="50"/>
+      <c r="M20" s="43"/>
       <c r="N20" s="7" t="s">
         <v>61</v>
       </c>
@@ -1740,10 +1740,10 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="38" t="s">
+      <c r="C24" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="38"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1752,10 +1752,10 @@
       <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="39" t="s">
+      <c r="D25" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="32" t="s">
         <v>61</v>
       </c>
@@ -1764,10 +1764,10 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="38"/>
+      <c r="J26" s="39"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1779,24 +1779,24 @@
       <c r="I27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="K27" s="40"/>
-      <c r="L27" s="39" t="s">
+      <c r="K27" s="41"/>
+      <c r="L27" s="40" t="s">
         <v>71</v>
       </c>
       <c r="M27" s="44"/>
-      <c r="N27" s="40"/>
+      <c r="N27" s="41"/>
       <c r="O27" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="38"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1805,10 +1805,10 @@
       <c r="C30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D30" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="37" t="s">
         <v>61</v>
       </c>
@@ -1817,10 +1817,10 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I31" s="38" t="s">
+      <c r="I31" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="J31" s="38"/>
+      <c r="J31" s="39"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
@@ -1832,10 +1832,10 @@
       <c r="I32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J32" s="39" t="s">
+      <c r="J32" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="40"/>
+      <c r="K32" s="41"/>
       <c r="L32" s="37" t="s">
         <v>61</v>
       </c>
@@ -2279,14 +2279,14 @@
       <c r="H100" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="I100" s="43" t="s">
+      <c r="I100" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="J100" s="43"/>
-      <c r="K100" s="41" t="s">
+      <c r="J100" s="50"/>
+      <c r="K100" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="L100" s="42"/>
+      <c r="L100" s="49"/>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
@@ -2300,16 +2300,26 @@
       <c r="B102" s="21">
         <v>87</v>
       </c>
-      <c r="C102" s="41" t="s">
+      <c r="C102" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="D102" s="42"/>
+      <c r="D102" s="49"/>
       <c r="F102" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2319,16 +2329,6 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="L20:M20"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="I100:J100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add time synchronisation to clock sync procedure
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DEB916-5DF0-4AAD-BDE2-9A4C774CCD2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E5D9FB-997D-4C6B-8F91-C3CEA29E0726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -231,15 +231,6 @@
     <t>Clock response</t>
   </si>
   <si>
-    <t>Origin clock (32 bits integer) T1</t>
-  </si>
-  <si>
-    <t>Receive clock (32 bits integer) T2</t>
-  </si>
-  <si>
-    <t>Transmit clock (32 bits integer) T3</t>
-  </si>
-  <si>
     <t>Registration finished</t>
   </si>
   <si>
@@ -343,6 +334,15 @@
   </si>
   <si>
     <t>Address (6 byte)*</t>
+  </si>
+  <si>
+    <t>Origin clock (64 bits integer) T1</t>
+  </si>
+  <si>
+    <t>Receive clock (64 bits integer) T2</t>
+  </si>
+  <si>
+    <t>Transmit clock (64 bits integer) T3</t>
   </si>
 </sst>
 </file>
@@ -830,9 +830,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -842,10 +839,13 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -860,13 +860,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1445,7 +1445,7 @@
   <dimension ref="B4:U102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1467,21 +1467,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="J4" s="38" t="s">
+      <c r="C4" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="J4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1502,7 +1502,7 @@
         <v>65</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>25</v>
@@ -1510,10 +1510,10 @@
       <c r="F6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="42"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1544,7 +1544,7 @@
         <v>65</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
@@ -1552,10 +1552,10 @@
       <c r="L8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="N8" s="49"/>
       <c r="O8" t="s">
         <v>63</v>
       </c>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
@@ -1597,12 +1597,12 @@
       <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="50"/>
+      <c r="I13" s="34" t="s">
         <v>87</v>
-      </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="34" t="s">
-        <v>90</v>
       </c>
       <c r="J13" s="35"/>
       <c r="K13" s="7" t="s">
@@ -1617,7 +1617,7 @@
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
@@ -1625,7 +1625,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>65</v>
@@ -1637,10 +1637,10 @@
         <v>5</v>
       </c>
       <c r="L15" s="36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="7" t="s">
@@ -1649,11 +1649,11 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2"/>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
@@ -1667,10 +1667,10 @@
         <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F17" s="45" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G17" s="46"/>
       <c r="H17" s="47"/>
@@ -1700,10 +1700,10 @@
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="43" t="s">
+      <c r="L20" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="M20" s="43"/>
+      <c r="M20" s="50"/>
       <c r="N20" s="7" t="s">
         <v>61</v>
       </c>
@@ -1740,10 +1740,10 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1752,10 +1752,10 @@
       <c r="C25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="41"/>
+      <c r="D25" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="40"/>
       <c r="F25" s="32" t="s">
         <v>61</v>
       </c>
@@ -1764,10 +1764,10 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="J26" s="39"/>
+      <c r="J26" s="38"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1779,36 +1779,36 @@
       <c r="I27" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J27" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="K27" s="41"/>
-      <c r="L27" s="40" t="s">
-        <v>71</v>
+      <c r="J27" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="K27" s="40"/>
+      <c r="L27" s="39" t="s">
+        <v>106</v>
       </c>
       <c r="M27" s="44"/>
-      <c r="N27" s="41"/>
+      <c r="N27" s="40"/>
       <c r="O27" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C29" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="39"/>
+      <c r="C29" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="40" t="s">
-        <v>95</v>
-      </c>
-      <c r="E30" s="41"/>
+      <c r="D30" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="40"/>
       <c r="F30" s="37" t="s">
         <v>61</v>
       </c>
@@ -1817,25 +1817,25 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="I31" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="39"/>
+      <c r="I31" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I32" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J32" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="K32" s="41"/>
+      <c r="J32" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="40"/>
       <c r="L32" s="37" t="s">
         <v>61</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="J33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.2">
@@ -1855,7 +1855,7 @@
     </row>
     <row r="37" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="3:21" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>28</v>
       </c>
       <c r="G82" s="26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H82" s="26"/>
       <c r="I82" s="26"/>
@@ -2202,12 +2202,12 @@
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>6</v>
@@ -2226,12 +2226,12 @@
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G93" s="10" t="s">
         <v>6</v>
@@ -2245,10 +2245,10 @@
         <v>86</v>
       </c>
       <c r="C94" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D94" s="25" t="s">
         <v>76</v>
-      </c>
-      <c r="D94" s="25" t="s">
-        <v>79</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>2</v>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.2">
@@ -2264,12 +2264,12 @@
         <v>6</v>
       </c>
       <c r="H97" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.2">
       <c r="H99" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.2">
@@ -2277,49 +2277,39 @@
         <v>6</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="I100" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="J100" s="50"/>
-      <c r="K100" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="L100" s="49"/>
+        <v>99</v>
+      </c>
+      <c r="I100" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="J100" s="43"/>
+      <c r="K100" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="L100" s="42"/>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I101" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B102" s="21">
         <v>87</v>
       </c>
-      <c r="C102" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="D102" s="49"/>
+      <c r="C102" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D102" s="42"/>
       <c r="F102" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="C29:D29"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2329,6 +2319,16 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="L20:M20"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="I100:J100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix protocol messages description
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630C0AA6-F55B-4AB3-B464-94DB0A88DC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B8AF9-A56E-4A4F-B516-CAE327FE9DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>Tag (16 byte)</t>
   </si>
   <si>
-    <t>Payload (up to 217 bytes)</t>
-  </si>
-  <si>
     <t>Tag is calculated using Poly1305 from last 8 bytes of Network Key</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>Payload (up to 214 bytes)</t>
+  </si>
+  <si>
+    <t>Payload (up to 215 bytes)</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -772,15 +772,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -802,7 +793,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -852,8 +843,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -861,16 +852,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -882,22 +873,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1476,7 +1458,7 @@
   <dimension ref="B4:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22:I22"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1498,21 +1480,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="J4" s="47" t="s">
+      <c r="C4" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="J4" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1530,10 +1512,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>25</v>
@@ -1541,22 +1523,22 @@
       <c r="F6" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="48"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J6" s="10"/>
       <c r="L6" s="10"/>
       <c r="O6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="10"/>
       <c r="I7" s="2" t="s">
@@ -1566,7 +1548,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1575,10 +1557,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="11" t="s">
         <v>5</v>
@@ -1586,12 +1568,12 @@
       <c r="L8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="48" t="s">
+      <c r="M8" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="48"/>
+      <c r="N8" s="37"/>
       <c r="O8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
@@ -1600,7 +1582,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L9" s="10"/>
     </row>
@@ -1614,7 +1596,7 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
@@ -1622,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>16</v>
@@ -1631,14 +1613,14 @@
         <v>5</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="49"/>
+        <v>106</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="43"/>
       <c r="I13" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J13" s="39"/>
       <c r="K13" s="7" t="s">
@@ -1648,12 +1630,12 @@
         <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
@@ -1661,10 +1643,10 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>16</v>
@@ -1673,27 +1655,27 @@
         <v>5</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="48" t="s">
+      <c r="P15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="48"/>
+      <c r="Q15" s="37"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2"/>
       <c r="I16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -1707,10 +1689,10 @@
         <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
@@ -1732,7 +1714,7 @@
         <v>28</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>16</v>
@@ -1741,16 +1723,16 @@
         <v>5</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="M20" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="N20" s="49"/>
-      <c r="O20" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="M20" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="N20" s="43"/>
+      <c r="O20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="48"/>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1763,7 +1745,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>16</v>
@@ -1772,13 +1754,13 @@
         <v>5</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="51"/>
-      <c r="I22" s="52"/>
+        <v>5</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
       <c r="J22" s="7" t="s">
         <v>61</v>
       </c>
@@ -1787,23 +1769,23 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="37"/>
+      <c r="C24" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="42"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25" s="39"/>
       <c r="G25" s="32" t="s">
@@ -1814,10 +1796,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="J26" s="37"/>
+      <c r="I26" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="42"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1827,42 +1809,42 @@
         <v>52</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K27" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L27" s="39"/>
       <c r="M27" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="N27" s="43"/>
-      <c r="O27" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="N27" s="40"/>
+      <c r="O27" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="48"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="37"/>
+      <c r="C29" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="42"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F30" s="39"/>
       <c r="G30" s="34" t="s">
@@ -1874,7 +1856,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I31" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J31" s="35"/>
     </row>
@@ -1883,16 +1865,16 @@
         <v>6</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K32" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L32" s="39"/>
       <c r="M32" s="36" t="s">
@@ -1904,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="K33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.2">
@@ -1914,7 +1896,7 @@
     </row>
     <row r="37" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="3:21" x14ac:dyDescent="0.2">
@@ -2165,7 +2147,7 @@
       <c r="G74" s="29"/>
       <c r="H74" s="30"/>
       <c r="I74" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J74" s="30"/>
       <c r="K74" s="31"/>
@@ -2223,7 +2205,7 @@
         <v>28</v>
       </c>
       <c r="G82" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H82" s="26"/>
       <c r="I82" s="26"/>
@@ -2261,12 +2243,12 @@
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G89" s="10" t="s">
         <v>6</v>
@@ -2285,12 +2267,12 @@
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G93" s="10" t="s">
         <v>6</v>
@@ -2304,10 +2286,10 @@
         <v>86</v>
       </c>
       <c r="C94" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D94" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>2</v>
@@ -2315,7 +2297,7 @@
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.2">
@@ -2323,12 +2305,12 @@
         <v>6</v>
       </c>
       <c r="H97" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
@@ -2336,48 +2318,46 @@
         <v>6</v>
       </c>
       <c r="H100" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="I100" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="J100" s="41"/>
+        <v>97</v>
+      </c>
+      <c r="I100" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="J100" s="48"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B102" s="21">
         <v>87</v>
       </c>
-      <c r="C102" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="D102" s="42"/>
-      <c r="E102" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="F102" s="41"/>
+      <c r="C102" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D102" s="49"/>
+      <c r="E102" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="F102" s="48"/>
       <c r="G102" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C103" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="C102:D102"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2387,13 +2367,15 @@
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="M20:N20"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
     <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="C102:D102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add counters to control messages
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9B8AF9-A56E-4A4F-B516-CAE327FE9DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21353169-C84B-456D-99F6-EDD23710030D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="111">
   <si>
     <t>FF</t>
   </si>
@@ -793,7 +793,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -807,7 +807,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -833,14 +832,16 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,6 +881,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1458,7 +1465,7 @@
   <dimension ref="B4:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1480,21 +1487,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="J4" s="41" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="J4" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="41"/>
-      <c r="O4" s="41"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1511,22 +1518,22 @@
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1556,22 +1563,22 @@
       <c r="H8" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="L8" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="37"/>
+      <c r="N8" s="36"/>
       <c r="O8" t="s">
         <v>62</v>
       </c>
@@ -1603,27 +1610,27 @@
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="43" t="s">
+      <c r="F13" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="43"/>
-      <c r="I13" s="38" t="s">
+      <c r="H13" s="42"/>
+      <c r="I13" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="39"/>
-      <c r="K13" s="7" t="s">
+      <c r="J13" s="38"/>
+      <c r="K13" s="34" t="s">
         <v>61</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -1645,29 +1652,29 @@
       <c r="H15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="8" t="s">
+      <c r="K15" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L15" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="M15" s="33" t="s">
+      <c r="M15" s="35" t="s">
         <v>82</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>109</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="37" t="s">
+      <c r="P15" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="37"/>
+      <c r="Q15" s="36"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1682,7 +1689,7 @@
       <c r="B17" s="9">
         <v>11</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="34" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1691,11 +1698,11 @@
       <c r="E17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1713,26 +1720,26 @@
       <c r="H20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="I20" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="M20" s="43" t="s">
+      <c r="M20" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="N20" s="43"/>
-      <c r="O20" s="37" t="s">
+      <c r="N20" s="42"/>
+      <c r="O20" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="37"/>
+      <c r="P20" s="36"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1744,24 +1751,24 @@
       <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="43" t="s">
+      <c r="F22" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="7" t="s">
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="34" t="s">
         <v>61</v>
       </c>
       <c r="K22" s="1" t="s">
@@ -1769,26 +1776,26 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="41"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="32" t="s">
+      <c r="F25" s="38"/>
+      <c r="G25" s="31" t="s">
         <v>61</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -1796,10 +1803,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="42" t="s">
+      <c r="I26" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="42"/>
+      <c r="J26" s="41"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1808,57 +1815,61 @@
       <c r="H27" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="I27" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="K27" s="38" t="s">
+      <c r="K27" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="39"/>
-      <c r="M27" s="38" t="s">
+      <c r="L27" s="38"/>
+      <c r="M27" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="40"/>
-      <c r="O27" s="37" t="s">
+      <c r="N27" s="39"/>
+      <c r="O27" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="37"/>
+      <c r="P27" s="36"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="42"/>
+      <c r="D29" s="41"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="F30" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="F30" s="39"/>
-      <c r="G30" s="34" t="s">
+      <c r="G30" s="38"/>
+      <c r="H30" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="36"/>
+      <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I31" s="35" t="s">
+      <c r="I31" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="J31" s="35"/>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
@@ -1867,17 +1878,17 @@
       <c r="H32" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I32" s="7" t="s">
+      <c r="I32" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="38" t="s">
+      <c r="K32" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="L32" s="39"/>
-      <c r="M32" s="36" t="s">
+      <c r="L32" s="38"/>
+      <c r="M32" s="33" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1911,7 +1922,7 @@
       <c r="H39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="34" t="s">
         <v>10</v>
       </c>
       <c r="R39" t="s">
@@ -1956,10 +1967,10 @@
       <c r="D43" s="4"/>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="12"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C45" s="3" t="s">
@@ -1973,129 +1984,128 @@
       </c>
       <c r="D46" s="5"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C49" s="13" t="s">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C49" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H52" s="15" t="s">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G52" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G53" s="10" t="s">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F53" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="G53" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="16"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="21">
+      <c r="H53" s="15"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="20">
         <v>81</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="1" t="s">
+      <c r="D54" s="50"/>
+      <c r="E54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H54" s="17"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H56" t="s">
+      <c r="G54" s="16"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G57" s="10" t="s">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F57" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="G57" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="20">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B58" s="19">
         <v>82</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="F58" s="1" t="s">
+      <c r="D58" s="22"/>
+      <c r="E58" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H60" t="s">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G61" s="10" t="s">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F61" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H61" s="19" t="s">
+      <c r="G61" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I61" s="22" t="s">
+      <c r="H61" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J61" s="23"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="20">
+      <c r="I61" s="22"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B62" s="19">
         <v>82</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="D62" s="23"/>
-      <c r="F62" s="1" t="s">
+      <c r="D62" s="22"/>
+      <c r="E62" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F63" s="1"/>
-      <c r="H63" t="s">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E63" s="1"/>
+      <c r="G63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="F64" s="1"/>
-      <c r="G64" s="10" t="s">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E64" s="1"/>
+      <c r="F64" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H64" s="18" t="s">
+      <c r="G64" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="66" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="H66" t="s">
+      <c r="G66" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G67" s="10" t="s">
+      <c r="F67" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H67" s="20" t="s">
+      <c r="G67" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I67" s="22" t="s">
+      <c r="H67" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="J67" s="24"/>
-      <c r="K67" s="24"/>
-      <c r="L67" s="23"/>
+      <c r="I67" s="23"/>
+      <c r="J67" s="23"/>
+      <c r="K67" s="22"/>
     </row>
     <row r="69" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="E69" s="13" t="s">
+      <c r="E69" s="12" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2103,33 +2113,33 @@
       <c r="D70" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="27" t="s">
+      <c r="E70" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F70" s="28"/>
-      <c r="G70" s="29" t="s">
+      <c r="F70" s="27"/>
+      <c r="G70" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H70" s="30"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29" t="s">
+      <c r="H70" s="29"/>
+      <c r="I70" s="28"/>
+      <c r="J70" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K70" s="30"/>
-      <c r="L70" s="29" t="s">
+      <c r="K70" s="29"/>
+      <c r="L70" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="M70" s="30"/>
-      <c r="N70" s="31"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="30"/>
     </row>
     <row r="72" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C72" s="14" t="s">
+      <c r="C72" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="21" t="s">
+      <c r="D72" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="E72" s="24" t="s">
         <v>41</v>
       </c>
       <c r="F72" s="1" t="s">
@@ -2140,26 +2150,26 @@
       <c r="D74" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="27" t="s">
+      <c r="E74" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F74" s="28"/>
-      <c r="G74" s="29"/>
-      <c r="H74" s="30"/>
-      <c r="I74" s="30" t="s">
+      <c r="F74" s="27"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="J74" s="30"/>
-      <c r="K74" s="31"/>
+      <c r="J74" s="29"/>
+      <c r="K74" s="30"/>
     </row>
     <row r="76" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D76" s="14" t="s">
+      <c r="D76" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E76" s="20" t="s">
+      <c r="E76" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F76" s="26" t="s">
+      <c r="F76" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G76" s="1" t="s">
@@ -2167,13 +2177,13 @@
       </c>
     </row>
     <row r="78" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D78" s="14" t="s">
+      <c r="D78" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E78" s="20" t="s">
+      <c r="E78" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="26" t="s">
+      <c r="F78" s="25" t="s">
         <v>24</v>
       </c>
       <c r="G78" s="1" t="s">
@@ -2181,13 +2191,13 @@
       </c>
     </row>
     <row r="80" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E80" s="20" t="s">
+      <c r="E80" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F80" s="26" t="s">
+      <c r="F80" s="25" t="s">
         <v>30</v>
       </c>
       <c r="G80" s="1" t="s">
@@ -2195,32 +2205,32 @@
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D82" s="14" t="s">
+      <c r="D82" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E82" s="20" t="s">
+      <c r="E82" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F82" s="26" t="s">
+      <c r="F82" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G82" s="26" t="s">
+      <c r="G82" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="H82" s="26"/>
-      <c r="I82" s="26"/>
+      <c r="H82" s="25"/>
+      <c r="I82" s="25"/>
       <c r="J82" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D84" s="14" t="s">
+      <c r="D84" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E84" s="21" t="s">
+      <c r="E84" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F84" s="25" t="s">
+      <c r="F84" s="24" t="s">
         <v>51</v>
       </c>
       <c r="G84" s="1" t="s">
@@ -2228,13 +2238,13 @@
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D86" s="14" t="s">
+      <c r="D86" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="E86" s="21" t="s">
+      <c r="E86" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="F86" s="25" t="s">
+      <c r="F86" s="24" t="s">
         <v>52</v>
       </c>
       <c r="G86" s="1" t="s">
@@ -2253,12 +2263,12 @@
       <c r="G89" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H89" s="18" t="s">
+      <c r="H89" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="21">
+      <c r="B90" s="20">
         <v>85</v>
       </c>
       <c r="F90" s="1" t="s">
@@ -2277,18 +2287,18 @@
       <c r="G93" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H93" s="18" t="s">
+      <c r="H93" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="21">
+      <c r="B94" s="20">
         <v>86</v>
       </c>
-      <c r="C94" s="25" t="s">
+      <c r="C94" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D94" s="25" t="s">
+      <c r="D94" s="24" t="s">
         <v>75</v>
       </c>
       <c r="F94" s="1" t="s">
@@ -2304,7 +2314,7 @@
       <c r="G97" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H97" s="18" t="s">
+      <c r="H97" s="17" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2317,13 +2327,13 @@
       <c r="G100" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H100" s="18" t="s">
+      <c r="H100" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I100" s="47" t="s">
+      <c r="I100" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="J100" s="48"/>
+      <c r="J100" s="47"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
@@ -2331,17 +2341,17 @@
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B102" s="21">
+      <c r="B102" s="20">
         <v>87</v>
       </c>
-      <c r="C102" s="49" t="s">
+      <c r="C102" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D102" s="49"/>
-      <c r="E102" s="47" t="s">
+      <c r="D102" s="48"/>
+      <c r="E102" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="F102" s="48"/>
+      <c r="F102" s="47"/>
       <c r="G102" s="1" t="s">
         <v>2</v>
       </c>
@@ -2352,12 +2362,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="E30:F30"/>
+  <mergeCells count="25">
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E102:F102"/>
     <mergeCell ref="I100:J100"/>
     <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2380,7 +2392,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I73 I75 H20 H52:H61 F76:F86 E72 H64 B25 H93 H89 B30 H32 H97 H100" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I73 I75 H20 F76:F86 E72 B25 H93 H89 B30 H32 H97 H100" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Implement restart node command
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB37D24-4320-48C7-97E1-371F33E8C508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C72651C-ED33-4960-B820-8B84702505B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
   <si>
     <t>FF</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Result Code:</t>
+  </si>
+  <si>
+    <t>Restart MCU</t>
+  </si>
+  <si>
+    <t>09</t>
   </si>
 </sst>
 </file>
@@ -850,14 +856,35 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,27 +896,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1465,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U103"/>
+  <dimension ref="B4:U105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1490,21 +1496,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="J4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1533,10 +1539,10 @@
       <c r="F6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="44"/>
+      <c r="H6" s="37"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1578,10 +1584,10 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="44"/>
+      <c r="N8" s="37"/>
       <c r="O8" t="s">
         <v>62</v>
       </c>
@@ -1625,14 +1631,14 @@
       <c r="F13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="46"/>
-      <c r="I13" s="37" t="s">
+      <c r="H13" s="38"/>
+      <c r="I13" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="34" t="s">
         <v>61</v>
       </c>
@@ -1674,10 +1680,10 @@
         <v>109</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="44"/>
+      <c r="Q15" s="37"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1701,11 +1707,11 @@
       <c r="E17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1735,14 +1741,14 @@
       <c r="L20" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="M20" s="46" t="s">
+      <c r="M20" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="N20" s="46"/>
-      <c r="O20" s="44" t="s">
+      <c r="N20" s="38"/>
+      <c r="O20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="44"/>
+      <c r="P20" s="37"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1766,11 +1772,11 @@
       <c r="F22" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="34" t="s">
         <v>61</v>
       </c>
@@ -1779,10 +1785,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="39" t="s">
+      <c r="C24" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1794,10 +1800,10 @@
       <c r="D25" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E25" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="31" t="s">
         <v>61</v>
       </c>
@@ -1806,10 +1812,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="39" t="s">
+      <c r="I26" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="39"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1824,24 +1830,24 @@
       <c r="J27" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="K27" s="37" t="s">
+      <c r="K27" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="38"/>
-      <c r="M27" s="37" t="s">
+      <c r="L27" s="40"/>
+      <c r="M27" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="50"/>
-      <c r="O27" s="44" t="s">
+      <c r="N27" s="41"/>
+      <c r="O27" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="44"/>
+      <c r="P27" s="37"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1856,14 +1862,14 @@
       <c r="E30" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="44" t="s">
+      <c r="G30" s="40"/>
+      <c r="H30" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I30" s="44"/>
+      <c r="I30" s="37"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1887,10 +1893,10 @@
       <c r="J32" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="K32" s="37" t="s">
+      <c r="K32" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="L32" s="38"/>
+      <c r="L32" s="40"/>
       <c r="M32" s="33" t="s">
         <v>61</v>
       </c>
@@ -2013,10 +2019,10 @@
       <c r="B54" s="20">
         <v>81</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="43"/>
+      <c r="D54" s="50"/>
       <c r="E54" s="1" t="s">
         <v>2</v>
       </c>
@@ -2336,10 +2342,10 @@
       <c r="H100" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I100" s="40" t="s">
+      <c r="I100" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="J100" s="41"/>
+      <c r="J100" s="48"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
@@ -2350,14 +2356,14 @@
       <c r="B102" s="20">
         <v>87</v>
       </c>
-      <c r="C102" s="42" t="s">
+      <c r="C102" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="D102" s="42"/>
-      <c r="E102" s="40" t="s">
+      <c r="D102" s="49"/>
+      <c r="E102" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="F102" s="41"/>
+      <c r="F102" s="48"/>
       <c r="G102" s="1" t="s">
         <v>2</v>
       </c>
@@ -2367,16 +2373,27 @@
         <v>98</v>
       </c>
     </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G105" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H105" s="17" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2387,18 +2404,20 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="F17:H17"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="H30:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I73 I75 H20 F76:F86 E72 B25 H93 H89 B30 H32 H97 H100 H27 G53:G64" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I73 I75 H20 F76:F86 E72 B25 H93 H89 B30 H32 H97 H100 H27 G53:G64 H105" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Document node MCU restart command
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C72651C-ED33-4960-B820-8B84702505B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5CDA08-D5D1-4FCF-B137-151907F5ADAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,10 +360,10 @@
     <t>Result Code:</t>
   </si>
   <si>
-    <t>Restart MCU</t>
-  </si>
-  <si>
     <t>09</t>
+  </si>
+  <si>
+    <t>Restart Node MCU</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1474,7 @@
   <dimension ref="B4:U105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I109" sqref="I109"/>
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2375,7 +2375,7 @@
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H104" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.2">
@@ -2383,7 +2383,7 @@
         <v>6</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement BroadcastKey message in gateway
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5CDA08-D5D1-4FCF-B137-151907F5ADAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ADA344-3BF0-43C7-B06C-D167015BD50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10755" yWindow="2535" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
   <si>
     <t>FF</t>
   </si>
@@ -364,6 +364,33 @@
   </si>
   <si>
     <t>Restart Node MCU</t>
+  </si>
+  <si>
+    <t>Random (32 bytes)</t>
+  </si>
+  <si>
+    <t>Request broadcast key</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Broadcast Key (32 bytes)</t>
+  </si>
+  <si>
+    <t>Send broadcast key</t>
+  </si>
+  <si>
+    <t>Counter 1: Data counter from node</t>
+  </si>
+  <si>
+    <t>Counter 2: Control data from node</t>
+  </si>
+  <si>
+    <t>Counter 3 (2 byte)</t>
+  </si>
+  <si>
+    <t>Counter 3: Counter for messages from gateway</t>
   </si>
 </sst>
 </file>
@@ -802,7 +829,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -862,29 +889,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -896,6 +902,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1471,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U105"/>
+  <dimension ref="B4:U113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1496,21 +1529,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="J4" s="42" t="s">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="J4" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1539,10 +1572,10 @@
       <c r="F6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="37"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1584,10 +1617,10 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="37"/>
+      <c r="N8" s="44"/>
       <c r="O8" t="s">
         <v>62</v>
       </c>
@@ -1629,16 +1662,16 @@
         <v>5</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="39" t="s">
+      <c r="H13" s="48"/>
+      <c r="I13" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="40"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="34" t="s">
         <v>61</v>
       </c>
@@ -1671,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="M15" s="35" t="s">
         <v>82</v>
@@ -1680,10 +1713,10 @@
         <v>109</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="37" t="s">
+      <c r="P15" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="37"/>
+      <c r="Q15" s="44"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1707,11 +1740,11 @@
       <c r="E17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="F17" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="46"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1739,16 +1772,16 @@
         <v>5</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="M20" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="M20" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="N20" s="38"/>
-      <c r="O20" s="37" t="s">
+      <c r="N20" s="48"/>
+      <c r="O20" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="37"/>
+      <c r="P20" s="44"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1770,13 +1803,13 @@
         <v>5</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="34" t="s">
         <v>61</v>
       </c>
@@ -1785,10 +1818,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="43"/>
+      <c r="D24" s="39"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1800,10 +1833,10 @@
       <c r="D25" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="40"/>
+      <c r="F25" s="47"/>
       <c r="G25" s="31" t="s">
         <v>61</v>
       </c>
@@ -1812,10 +1845,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="43"/>
+      <c r="J26" s="39"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1828,26 +1861,26 @@
         <v>64</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="K27" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K27" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="40"/>
-      <c r="M27" s="39" t="s">
+      <c r="L27" s="47"/>
+      <c r="M27" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="41"/>
-      <c r="O27" s="37" t="s">
+      <c r="N27" s="52"/>
+      <c r="O27" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="37"/>
+      <c r="P27" s="44"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="39"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1862,14 +1895,14 @@
       <c r="E30" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="40"/>
-      <c r="H30" s="37" t="s">
+      <c r="G30" s="47"/>
+      <c r="H30" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="I30" s="37"/>
+      <c r="I30" s="44"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1891,20 +1924,18 @@
         <v>64</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="K32" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="L32" s="40"/>
+      <c r="L32" s="47"/>
       <c r="M32" s="33" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>19</v>
-      </c>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G33" s="10"/>
       <c r="I33" t="s">
         <v>111</v>
       </c>
@@ -1912,470 +1943,495 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C34" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="39"/>
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="47"/>
+      <c r="G35" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="44"/>
+      <c r="I35" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G36" s="10"/>
+      <c r="I36" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="J36" s="39"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I37" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="J37" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="K37" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="L37" s="47"/>
+      <c r="M37" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="N37" s="44"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
+      <c r="F42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I38" s="2" t="s">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I46" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="F39" s="1" t="s">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I39" s="34" t="s">
+      <c r="I47" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R47" t="s">
         <v>12</v>
       </c>
-      <c r="S39">
+      <c r="S47">
         <v>6</v>
       </c>
-      <c r="T39">
+      <c r="T47">
         <v>2</v>
       </c>
-      <c r="U39">
+      <c r="U47">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>20</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I48" t="s">
         <v>11</v>
       </c>
-      <c r="S40" t="s">
+      <c r="S48" t="s">
         <v>13</v>
       </c>
-      <c r="T40" t="s">
+      <c r="T48" t="s">
         <v>14</v>
       </c>
-      <c r="U40" t="s">
+      <c r="U48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I41" t="s">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C43" s="4" t="s">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C51" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C44" s="11" t="s">
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C52" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="11"/>
-    </row>
-    <row r="45" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C45" s="3" t="s">
+      <c r="D52" s="11"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C46" s="5" t="s">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C54" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C49" s="12" t="s">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C57" s="12" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G52" s="14" t="s">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G60" s="14" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F53" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G53" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" s="15"/>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="20">
-        <v>81</v>
-      </c>
-      <c r="C54" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D54" s="50"/>
-      <c r="E54" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G54" s="16"/>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F57" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="19">
-        <v>82</v>
-      </c>
-      <c r="C58" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G60" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="F61" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H61" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="I61" s="22"/>
+      <c r="G61" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H61" s="15"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B62" s="19">
-        <v>82</v>
-      </c>
-      <c r="C62" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D62" s="22"/>
+      <c r="B62" s="20">
+        <v>81</v>
+      </c>
+      <c r="C62" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D62" s="43"/>
       <c r="E62" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E63" s="1"/>
-      <c r="G63" t="s">
+      <c r="G62" s="16"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B66" s="19">
+        <v>82</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F69" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H69" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="I69" s="22"/>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B70" s="19">
+        <v>82</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="22"/>
+      <c r="E70" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E71" s="1"/>
+      <c r="G71" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="E64" s="1"/>
-      <c r="F64" s="10" t="s">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E72" s="1"/>
+      <c r="F72" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G72" s="17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="G66" t="s">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="F67" s="10" t="s">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F75" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="19" t="s">
+      <c r="G75" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H67" s="21" t="s">
+      <c r="H75" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="22"/>
-    </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="E69" s="12" t="s">
+      <c r="I75" s="23"/>
+      <c r="J75" s="23"/>
+      <c r="K75" s="22"/>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E77" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D70" s="10" t="s">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D78" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E70" s="26" t="s">
+      <c r="E78" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="F70" s="27"/>
-      <c r="G70" s="28" t="s">
+      <c r="F78" s="27"/>
+      <c r="G78" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28" t="s">
+      <c r="H78" s="29"/>
+      <c r="I78" s="28"/>
+      <c r="J78" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K70" s="29"/>
-      <c r="L70" s="28" t="s">
+      <c r="K78" s="29"/>
+      <c r="L78" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="M70" s="29"/>
-      <c r="N70" s="30"/>
-    </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C72" s="13" t="s">
+      <c r="M78" s="29"/>
+      <c r="N78" s="30"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C80" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D80" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E72" s="24" t="s">
+      <c r="E80" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D74" s="10" t="s">
+    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D82" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E82" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F74" s="27"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="29"/>
-      <c r="I74" s="29" t="s">
+      <c r="F82" s="27"/>
+      <c r="G82" s="28"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="J74" s="29"/>
-      <c r="K74" s="30"/>
-    </row>
-    <row r="76" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D76" s="13" t="s">
+      <c r="J82" s="29"/>
+      <c r="K82" s="30"/>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D84" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E84" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F76" s="25" t="s">
+      <c r="F84" s="25" t="s">
         <v>7</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D78" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D80" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D82" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F82" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G82" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="H82" s="25"/>
-      <c r="I82" s="25"/>
-      <c r="J82" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D84" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>51</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D86" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E86" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F86" s="24" t="s">
-        <v>52</v>
+      <c r="F86" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="G86" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H88" t="s">
+    <row r="88" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D88" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D90" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G90" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H90" s="25"/>
+      <c r="I90" s="25"/>
+      <c r="J90" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D92" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D94" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B89" t="s">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
         <v>77</v>
       </c>
-      <c r="G89" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H89" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B90" s="20">
-        <v>85</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H92" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
-        <v>74</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H93" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="20">
-        <v>86</v>
-      </c>
-      <c r="C94" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D94" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H96" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
       <c r="G97" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H99" t="s">
-        <v>96</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B98" s="20">
+        <v>85</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G100" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H100" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="I100" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="J100" s="48"/>
+      <c r="H100" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>100</v>
+        <v>74</v>
+      </c>
+      <c r="G101" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="17" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B102" s="20">
-        <v>87</v>
-      </c>
-      <c r="C102" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="D102" s="49"/>
-      <c r="E102" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F102" s="48"/>
-      <c r="G102" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F102" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C103" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H104" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.2">
@@ -2383,17 +2439,80 @@
         <v>6</v>
       </c>
       <c r="H105" s="17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G108" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H108" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I108" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="J108" s="41"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B110" s="20">
+        <v>87</v>
+      </c>
+      <c r="C110" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D110" s="42"/>
+      <c r="E110" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F110" s="41"/>
+      <c r="G110" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C111" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G113" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H113" s="17" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="H30:I30"/>
+  <mergeCells count="31">
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2404,20 +2523,19 @@
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="F17:H17"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="I108:J108"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I73 I75 H20 F76:F86 E72 B25 H93 H89 B30 H32 H97 H100 H27 G53:G64 H105" numberStoredAsText="1"/>
+    <ignoredError sqref="B13 B21:B22 I81 I83 H20 F84:F94 E80 B25 H101 H97 B30 H32 H105 H108 H27 G61:G72 H113 B35 H37" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add broadcast flag to data/control messages sent from gateway
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ADA344-3BF0-43C7-B06C-D167015BD50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783F2DE-BC71-4C3D-A8F3-75BBB368A8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10755" yWindow="2535" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6315" yWindow="2280" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
   <si>
     <t>FF</t>
   </si>
@@ -345,9 +345,6 @@
     <t>Counter 1 (2 byte)</t>
   </si>
   <si>
-    <t>Counter 1 | Counter 2</t>
-  </si>
-  <si>
     <t>Counter 2 (2 byte)</t>
   </si>
   <si>
@@ -391,6 +388,12 @@
   </si>
   <si>
     <t>Counter 3: Counter for messages from gateway</t>
+  </si>
+  <si>
+    <t>NodeID (15 bits)</t>
+  </si>
+  <si>
+    <t>Broadcast (1 bit)</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -889,8 +892,38 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -902,33 +935,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1506,8 +1512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1528,24 +1534,24 @@
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="45" t="s">
+    <row r="4" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="C4" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="J4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1556,7 +1562,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1572,10 +1578,10 @@
       <c r="F6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="44"/>
+      <c r="H6" s="42"/>
       <c r="I6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1591,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>105</v>
       </c>
@@ -1595,7 +1601,7 @@
       </c>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>68</v>
       </c>
@@ -1617,25 +1623,23 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N8" s="44"/>
+      <c r="N8" s="42"/>
       <c r="O8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="K9" s="10"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1643,12 +1647,12 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
@@ -1658,36 +1662,39 @@
       <c r="D13" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>5</v>
+      <c r="E13" s="39" t="s">
+        <v>123</v>
       </c>
       <c r="F13" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="H13" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="44"/>
+      <c r="J13" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="47"/>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="41"/>
+      <c r="L13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G15" s="10" t="s">
         <v>6</v>
       </c>
@@ -1700,25 +1707,28 @@
       <c r="J15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="L15" s="35" t="s">
-        <v>121</v>
+      <c r="K15" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="39" t="s">
+        <v>122</v>
       </c>
       <c r="M15" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="N15" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="N15" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="O15" s="8"/>
-      <c r="P15" s="44" t="s">
+      <c r="O15" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="44"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R15" s="42"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
@@ -1727,7 +1737,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
         <v>11</v>
       </c>
@@ -1740,22 +1750,22 @@
       <c r="E17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G20" s="10" t="s">
         <v>6</v>
       </c>
@@ -1768,28 +1778,31 @@
       <c r="J20" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="M20" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="N20" s="48"/>
-      <c r="O20" s="44" t="s">
+      <c r="K20" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="L20" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="44"/>
+      <c r="P20" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="P20" s="44"/>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="Q20" s="42"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
@@ -1799,17 +1812,17 @@
       <c r="D22" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="39" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="G22" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
+        <v>107</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
       <c r="J22" s="34" t="s">
         <v>61</v>
       </c>
@@ -1817,13 +1830,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="39" t="s">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C24" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="39"/>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D24" s="43"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>51</v>
       </c>
@@ -1831,12 +1844,12 @@
         <v>64</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="47"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="31" t="s">
         <v>61</v>
       </c>
@@ -1844,13 +1857,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="39" t="s">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="I26" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="J26" s="43"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
         <v>6</v>
       </c>
@@ -1861,28 +1874,28 @@
         <v>64</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="K27" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="K27" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="L27" s="47"/>
-      <c r="M27" s="46" t="s">
+      <c r="L27" s="41"/>
+      <c r="M27" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="N27" s="52"/>
-      <c r="O27" s="44" t="s">
+      <c r="N27" s="45"/>
+      <c r="O27" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="P27" s="44"/>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="39" t="s">
+      <c r="P27" s="42"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C29" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D29" s="43"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
         <v>88</v>
       </c>
@@ -1893,27 +1906,27 @@
         <v>5</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="44" t="s">
+      <c r="G30" s="41"/>
+      <c r="H30" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="I30" s="44"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I31" s="32" t="s">
         <v>92</v>
       </c>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
         <v>6</v>
       </c>
@@ -1924,12 +1937,12 @@
         <v>64</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>121</v>
-      </c>
-      <c r="K32" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="K32" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="L32" s="47"/>
+      <c r="L32" s="41"/>
       <c r="M32" s="33" t="s">
         <v>61</v>
       </c>
@@ -1937,17 +1950,17 @@
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G33" s="10"/>
       <c r="I33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J33" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C34" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="D34" s="39"/>
+      <c r="C34" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="43"/>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
@@ -1958,48 +1971,48 @@
         <v>64</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="41"/>
+      <c r="G35" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="44"/>
+      <c r="H35" s="42"/>
       <c r="I35" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G36" s="10"/>
-      <c r="I36" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="J36" s="39"/>
+      <c r="I36" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G37" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I37" s="37" t="s">
         <v>64</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="K37" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="L37" s="47"/>
-      <c r="M37" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="K37" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="L37" s="41"/>
+      <c r="M37" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N37" s="44"/>
+      <c r="N37" s="42"/>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G38" s="10"/>
@@ -2009,7 +2022,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G40" s="10"/>
     </row>
@@ -2018,7 +2031,7 @@
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.2">
@@ -2026,7 +2039,7 @@
         <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.2">
@@ -2131,10 +2144,10 @@
       <c r="B62" s="20">
         <v>81</v>
       </c>
-      <c r="C62" s="43" t="s">
+      <c r="C62" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="D62" s="43"/>
+      <c r="D62" s="53"/>
       <c r="E62" s="1" t="s">
         <v>2</v>
       </c>
@@ -2454,10 +2467,10 @@
       <c r="H108" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="I108" s="40" t="s">
+      <c r="I108" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="J108" s="41"/>
+      <c r="J108" s="51"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
@@ -2468,14 +2481,14 @@
       <c r="B110" s="20">
         <v>87</v>
       </c>
-      <c r="C110" s="42" t="s">
+      <c r="C110" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="D110" s="42"/>
-      <c r="E110" s="40" t="s">
+      <c r="D110" s="52"/>
+      <c r="E110" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="F110" s="41"/>
+      <c r="F110" s="51"/>
       <c r="G110" s="1" t="s">
         <v>2</v>
       </c>
@@ -2487,7 +2500,7 @@
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H112" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="7:8" x14ac:dyDescent="0.2">
@@ -2495,34 +2508,11 @@
         <v>6</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="J4:O4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E110:F110"/>
     <mergeCell ref="I108:J108"/>
@@ -2531,6 +2521,29 @@
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="G35:H35"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="J4:O4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="F30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Move broadcast flag to message type (Gateway)
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2783F2DE-BC71-4C3D-A8F3-75BBB368A8F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2DA17B-95AC-47DE-A2F6-7E4372790486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6315" yWindow="2280" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="127">
   <si>
     <t>FF</t>
   </si>
@@ -282,12 +282,6 @@
     <t>Node Data (up to 214 bytes)</t>
   </si>
   <si>
-    <t>02/03</t>
-  </si>
-  <si>
-    <t>02 = SET command, 03 = GET command</t>
-  </si>
-  <si>
     <t>07</t>
   </si>
   <si>
@@ -390,10 +384,25 @@
     <t>Counter 3: Counter for messages from gateway</t>
   </si>
   <si>
-    <t>NodeID (15 bits)</t>
-  </si>
-  <si>
-    <t>Broadcast (1 bit)</t>
+    <t>04/84</t>
+  </si>
+  <si>
+    <t>84 = broadcast</t>
+  </si>
+  <si>
+    <t>01/81</t>
+  </si>
+  <si>
+    <t>02 = SET command, 12 = GET command</t>
+  </si>
+  <si>
+    <t>02/12/82/92</t>
+  </si>
+  <si>
+    <t>82/92 Broadcast</t>
+  </si>
+  <si>
+    <t>81 = broadcast</t>
   </si>
 </sst>
 </file>
@@ -1513,18 +1522,18 @@
   <dimension ref="B4:U113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1534,7 +1543,7 @@
     <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
       <c r="C4" s="46" t="s">
         <v>78</v>
       </c>
@@ -1551,7 +1560,7 @@
       <c r="N4" s="46"/>
       <c r="O4" s="46"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1562,7 +1571,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1591,9 +1600,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" s="10"/>
       <c r="I7" s="2" t="s">
@@ -1601,7 +1610,7 @@
       </c>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>68</v>
       </c>
@@ -1631,7 +1640,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -1639,7 +1648,7 @@
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1647,14 +1656,14 @@
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>64</v>
@@ -1663,43 +1672,43 @@
         <v>16</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="44"/>
-      <c r="J13" s="40" t="s">
+      <c r="H13" s="44"/>
+      <c r="I13" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="41"/>
-      <c r="L13" s="34" t="s">
+      <c r="J13" s="41"/>
+      <c r="K13" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P13" t="s">
+      <c r="O13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
       <c r="I14" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="G15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="I15" s="34" t="s">
         <v>64</v>
@@ -1708,36 +1717,36 @@
         <v>16</v>
       </c>
       <c r="K15" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>122</v>
+        <v>5</v>
+      </c>
+      <c r="L15" s="35" t="s">
+        <v>118</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="N15" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="O15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="42" t="s">
+      <c r="N15" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="R15" s="42"/>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q15" s="42"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D16" s="2"/>
+      <c r="G16" t="s">
+        <v>125</v>
+      </c>
       <c r="I16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
         <v>11</v>
       </c>
@@ -1759,18 +1768,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G20" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>28</v>
+        <v>120</v>
       </c>
       <c r="I20" s="34" t="s">
         <v>64</v>
@@ -1779,30 +1788,30 @@
         <v>16</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="L20" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="M20" s="35" t="s">
-        <v>120</v>
-      </c>
-      <c r="N20" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O20" s="44"/>
-      <c r="P20" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="M20" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="N20" s="44"/>
+      <c r="O20" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="Q20" s="42"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P20" s="42"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>30</v>
       </c>
@@ -1816,10 +1825,10 @@
         <v>5</v>
       </c>
       <c r="F22" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="44" t="s">
         <v>107</v>
-      </c>
-      <c r="G22" s="44" t="s">
-        <v>109</v>
       </c>
       <c r="H22" s="44"/>
       <c r="I22" s="44"/>
@@ -1830,13 +1839,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C24" s="43" t="s">
         <v>66</v>
       </c>
       <c r="D24" s="43"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
         <v>51</v>
       </c>
@@ -1844,10 +1853,10 @@
         <v>64</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E25" s="40" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F25" s="41"/>
       <c r="G25" s="31" t="s">
@@ -1857,13 +1866,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I26" s="43" t="s">
         <v>67</v>
       </c>
       <c r="J26" s="43"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
         <v>6</v>
       </c>
@@ -1874,14 +1883,14 @@
         <v>64</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K27" s="40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L27" s="41"/>
       <c r="M27" s="40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N27" s="45"/>
       <c r="O27" s="42" t="s">
@@ -1889,15 +1898,15 @@
       </c>
       <c r="P27" s="42"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C29" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="43"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>64</v>
@@ -1906,10 +1915,10 @@
         <v>5</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G30" s="41"/>
       <c r="H30" s="42" t="s">
@@ -1920,27 +1929,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I31" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I32" s="34" t="s">
         <v>64</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K32" s="40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L32" s="41"/>
       <c r="M32" s="33" t="s">
@@ -1950,31 +1959,31 @@
     <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G33" s="10"/>
       <c r="I33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J33" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C34" s="43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D34" s="43"/>
       <c r="G34" s="10"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B35" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35" s="37" t="s">
         <v>64</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" s="40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="42" t="s">
@@ -1988,7 +1997,7 @@
     <row r="36" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G36" s="10"/>
       <c r="I36" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J36" s="43"/>
     </row>
@@ -1997,16 +2006,16 @@
         <v>6</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I37" s="37" t="s">
         <v>64</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K37" s="40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L37" s="41"/>
       <c r="M37" s="42" t="s">
@@ -2022,7 +2031,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="F40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G40" s="10"/>
     </row>
@@ -2031,7 +2040,7 @@
         <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.2">
@@ -2039,7 +2048,7 @@
         <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.2">
@@ -2444,7 +2453,7 @@
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H104" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.2">
@@ -2452,12 +2461,12 @@
         <v>6</v>
       </c>
       <c r="H105" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H107" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.2">
@@ -2465,16 +2474,16 @@
         <v>6</v>
       </c>
       <c r="H108" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I108" s="50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J108" s="51"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.2">
@@ -2482,11 +2491,11 @@
         <v>87</v>
       </c>
       <c r="C110" s="52" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D110" s="52"/>
       <c r="E110" s="50" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F110" s="51"/>
       <c r="G110" s="1" t="s">
@@ -2495,12 +2504,12 @@
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C111" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H112" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="7:8" x14ac:dyDescent="0.2">
@@ -2508,7 +2517,7 @@
         <v>6</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2528,10 +2537,10 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="M8:N8"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="I13:J13"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="M27:N27"/>
     <mergeCell ref="O27:P27"/>
@@ -2540,15 +2549,15 @@
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="F30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B13 B21:B22 I81 I83 H20 F84:F94 E80 B25 H101 H97 B30 H32 H105 H108 H27 G61:G72 H113 B35 H37" numberStoredAsText="1"/>
+    <ignoredError sqref="B21:B22 I81 I83 F84:F94 E80 B25 H101 H97 B30 H32 H105 H108 H27 G61:G72 H113 B35 H37" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Send broadcast key in a control message
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8390CB52-4C08-47F2-A789-20865F19B708}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ED9368-63BF-474F-A030-797184B55D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="3705" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="125">
   <si>
     <t>FF</t>
   </si>
@@ -348,18 +348,6 @@
     <t>Restart Node MCU</t>
   </si>
   <si>
-    <t>Random (32 bytes)</t>
-  </si>
-  <si>
-    <t>Request broadcast key</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Broadcast Key (32 bytes)</t>
-  </si>
-  <si>
     <t>Send broadcast key</t>
   </si>
   <si>
@@ -396,9 +384,6 @@
     <t>TODO: Encrypt using network key, adding some random data. This is to avoid DoS attack. I have to investigate if this may really work</t>
   </si>
   <si>
-    <t>NOT IMPLEMENTED</t>
-  </si>
-  <si>
     <t>Sent just after registration</t>
   </si>
   <si>
@@ -406,6 +391,12 @@
   </si>
   <si>
     <t>Other options: mark message using timestamp. Adding a number calculated from node message (a byte should be sufficient). For instance nth byte + 3</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>Broadcast key (32 byte)</t>
   </si>
 </sst>
 </file>
@@ -844,7 +835,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -898,43 +889,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -947,6 +902,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1522,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U114"/>
+  <dimension ref="B4:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1547,21 +1532,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="J4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1585,18 +1570,18 @@
         <v>67</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="40"/>
+      <c r="I6" s="42"/>
       <c r="J6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1634,10 +1619,10 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="40"/>
+      <c r="N8" s="42"/>
       <c r="O8" t="s">
         <v>60</v>
       </c>
@@ -1673,20 +1658,20 @@
       <c r="D13" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="37" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="47" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42" t="s">
+      <c r="H13" s="47"/>
+      <c r="I13" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="J13" s="43"/>
+      <c r="J13" s="45"/>
       <c r="K13" s="34" t="s">
         <v>59</v>
       </c>
@@ -1707,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I15" s="34" t="s">
         <v>62</v>
@@ -1715,11 +1700,11 @@
       <c r="J15" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="37" t="s">
         <v>5</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="M15" s="35" t="s">
         <v>80</v>
@@ -1728,10 +1713,10 @@
         <v>103</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="40" t="s">
+      <c r="P15" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="Q15" s="40"/>
+      <c r="Q15" s="42"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1739,7 +1724,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="H16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -1755,11 +1740,11 @@
       <c r="E17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="50"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1775,7 +1760,7 @@
         <v>6</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I20" s="34" t="s">
         <v>62</v>
@@ -1783,20 +1768,20 @@
       <c r="J20" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="39" t="s">
+      <c r="K20" s="37" t="s">
         <v>5</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="M20" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="M20" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="N20" s="41"/>
-      <c r="O20" s="40" t="s">
+      <c r="N20" s="47"/>
+      <c r="O20" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="P20" s="40"/>
+      <c r="P20" s="42"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1804,7 +1789,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="H21" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
@@ -1817,17 +1802,17 @@
       <c r="D22" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="37" t="s">
         <v>5</v>
       </c>
       <c r="F22" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
       <c r="J22" s="34" t="s">
         <v>59</v>
       </c>
@@ -1836,10 +1821,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="46"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1851,10 +1836,10 @@
       <c r="D25" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="43"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="31" t="s">
         <v>59</v>
       </c>
@@ -1863,10 +1848,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="J26" s="46"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1879,26 +1864,26 @@
         <v>62</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="K27" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="K27" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="42" t="s">
+      <c r="L27" s="45"/>
+      <c r="M27" s="44" t="s">
         <v>100</v>
       </c>
-      <c r="N27" s="44"/>
-      <c r="O27" s="40" t="s">
+      <c r="N27" s="51"/>
+      <c r="O27" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="P27" s="40"/>
+      <c r="P27" s="42"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="46"/>
+      <c r="D29" s="43"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1913,14 +1898,14 @@
       <c r="E30" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="40" t="s">
+      <c r="G30" s="45"/>
+      <c r="H30" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="40"/>
+      <c r="I30" s="42"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1942,17 +1927,17 @@
         <v>62</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="K32" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="K32" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="L32" s="43"/>
+      <c r="L32" s="45"/>
       <c r="M32" s="33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:21" x14ac:dyDescent="0.2">
       <c r="G33" s="10"/>
       <c r="I33" t="s">
         <v>105</v>
@@ -1961,593 +1946,544 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C34" s="46" t="s">
+    <row r="34" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="46"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B35" s="9" t="s">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="J42" t="s">
+        <v>119</v>
+      </c>
+      <c r="R42" t="s">
+        <v>12</v>
+      </c>
+      <c r="S42">
+        <v>6</v>
+      </c>
+      <c r="T42">
+        <v>2</v>
+      </c>
+      <c r="U42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="F43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="J43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="S44" t="s">
+        <v>13</v>
+      </c>
+      <c r="T44" t="s">
+        <v>14</v>
+      </c>
+      <c r="U44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C47" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="3:21" x14ac:dyDescent="0.2">
+      <c r="C48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C50" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="5"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C53" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G56" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F57" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="20">
+        <v>81</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="41"/>
+      <c r="E58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G58" s="16"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F61" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="19">
+        <v>82</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="22"/>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B66" s="19">
+        <v>82</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E67" s="1"/>
+      <c r="G67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E68" s="1"/>
+      <c r="F68" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F71" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H71" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
+      <c r="K71" s="22"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E73" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D74" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F74" s="27"/>
+      <c r="G74" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="H74" s="29"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K74" s="29"/>
+      <c r="L74" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="M74" s="29"/>
+      <c r="N74" s="30"/>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C76" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D78" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F78" s="27"/>
+      <c r="G78" s="28"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="J78" s="29"/>
+      <c r="K78" s="30"/>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D80" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F80" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D82" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F82" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D84" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F84" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D86" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F86" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H86" s="25"/>
+      <c r="I86" s="25"/>
+      <c r="J86" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D88" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D90" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E90" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>75</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B94" s="20">
+        <v>85</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" t="s">
+        <v>72</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H97" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="20">
+        <v>86</v>
+      </c>
+      <c r="C98" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G101" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G104" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H104" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="H35" s="40"/>
-      <c r="I35" s="1" t="s">
+      <c r="I104" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="J104" s="39"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B105" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B106" s="20">
+        <v>87</v>
+      </c>
+      <c r="C106" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D106" s="40"/>
+      <c r="E106" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F106" s="39"/>
+      <c r="G106" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C36" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="I36" s="46" t="s">
-        <v>112</v>
-      </c>
-      <c r="J36" s="46"/>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G37" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="I37" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="J37" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="K37" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="L37" s="43"/>
-      <c r="M37" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="N37" s="40"/>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G38" s="10"/>
-      <c r="I38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F40" t="s">
-        <v>113</v>
-      </c>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I46" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I47" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="J47" t="s">
-        <v>123</v>
-      </c>
-      <c r="R47" t="s">
-        <v>12</v>
-      </c>
-      <c r="S47">
-        <v>6</v>
-      </c>
-      <c r="T47">
-        <v>2</v>
-      </c>
-      <c r="U47">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="J48" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>20</v>
-      </c>
-      <c r="I49" t="s">
-        <v>11</v>
-      </c>
-      <c r="S49" t="s">
-        <v>13</v>
-      </c>
-      <c r="T49" t="s">
-        <v>14</v>
-      </c>
-      <c r="U49" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="I50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C52" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="4"/>
-      <c r="E52" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C53" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="11"/>
-    </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C54" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C55" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C58" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="G61" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="F62" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" s="15"/>
-    </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B63" s="20">
-        <v>81</v>
-      </c>
-      <c r="C63" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="D63" s="53"/>
-      <c r="E63" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G63" s="16"/>
-    </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F66" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G66" s="17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B67" s="19">
-        <v>82</v>
-      </c>
-      <c r="C67" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G69" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F70" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H70" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="I70" s="22"/>
-    </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B71" s="19">
-        <v>82</v>
-      </c>
-      <c r="C71" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D71" s="22"/>
-      <c r="E71" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E72" s="1"/>
-      <c r="G72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E73" s="1"/>
-      <c r="F73" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G73" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G75" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F76" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G76" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="H76" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="I76" s="23"/>
-      <c r="J76" s="23"/>
-      <c r="K76" s="22"/>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E78" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D79" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F79" s="27"/>
-      <c r="G79" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="H79" s="29"/>
-      <c r="I79" s="28"/>
-      <c r="J79" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="K79" s="29"/>
-      <c r="L79" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="M79" s="29"/>
-      <c r="N79" s="30"/>
-    </row>
-    <row r="81" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C81" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D83" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="F83" s="27"/>
-      <c r="G83" s="28"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="J83" s="29"/>
-      <c r="K83" s="30"/>
-    </row>
-    <row r="85" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D85" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F85" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D87" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E87" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F87" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D89" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F89" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D91" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G91" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
-      <c r="J91" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D93" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F93" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="D95" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E95" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="F95" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H97" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B98" t="s">
-        <v>75</v>
-      </c>
-      <c r="G98" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H98" s="17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B99" s="20">
-        <v>85</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H101" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B102" t="s">
-        <v>72</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H102" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B103" s="20">
-        <v>86</v>
-      </c>
-      <c r="C103" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D103" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H105" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G106" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H106" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C107" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H108" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="G109" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="I109" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="J109" s="51"/>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B110" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B111" s="20">
-        <v>87</v>
-      </c>
-      <c r="C111" s="52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D111" s="52"/>
-      <c r="E111" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="F111" s="51"/>
-      <c r="G111" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="C112" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="113" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="H113" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="114" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G114" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G112" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H114" s="17" t="s">
-        <v>106</v>
+      <c r="H112" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="I112" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="J112" s="39"/>
+      <c r="K112" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="I109:J109"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="M37:N37"/>
+  <mergeCells count="26">
+    <mergeCell ref="I112:J112"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2560,19 +2496,16 @@
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="I104:J104"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="H30:I30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B21:B22 I82 I84 F85:F95 E81 B25 H102 H98 B30 H32 H106 H109 H27 G62:G73 H114 B35 H37 B13" numberStoredAsText="1"/>
+    <ignoredError sqref="B21:B22 I77 I79 F80:F90 E76 B25 H97 H93 B30 H32 H101 H104 H27 G57:G68 H109 B13" numberStoredAsText="1"/>
     <ignoredError sqref="H20" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>

</xml_diff>

<commit_message>
Implement restart notification control message from node
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ED9368-63BF-474F-A030-797184B55D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCB5F36-E4E5-41DD-AB3D-3FDEB8BA690A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5070" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
   <si>
     <t>FF</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Broadcast key (32 byte)</t>
+  </si>
+  <si>
+    <t>Restart confirm</t>
+  </si>
+  <si>
+    <t>Sent on intentional restart</t>
   </si>
 </sst>
 </file>
@@ -898,17 +904,11 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,11 +916,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,7 +934,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1509,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K110" sqref="K110"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1532,21 +1538,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="J4" s="46" t="s">
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="J4" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1578,10 +1584,10 @@
       <c r="G6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="42" t="s">
+      <c r="H6" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="40"/>
       <c r="J6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1619,10 +1625,10 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="42" t="s">
+      <c r="M8" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="42"/>
+      <c r="N8" s="40"/>
       <c r="O8" t="s">
         <v>60</v>
       </c>
@@ -1664,14 +1670,14 @@
       <c r="F13" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="47"/>
-      <c r="I13" s="44" t="s">
+      <c r="H13" s="41"/>
+      <c r="I13" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="J13" s="45"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="34" t="s">
         <v>59</v>
       </c>
@@ -1713,10 +1719,10 @@
         <v>103</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="42" t="s">
+      <c r="P15" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="Q15" s="42"/>
+      <c r="Q15" s="40"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1740,11 +1746,11 @@
       <c r="E17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="50"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1774,14 +1780,14 @@
       <c r="L20" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="M20" s="47" t="s">
+      <c r="M20" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="N20" s="47"/>
-      <c r="O20" s="42" t="s">
+      <c r="N20" s="41"/>
+      <c r="O20" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="P20" s="42"/>
+      <c r="P20" s="40"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1808,11 +1814,11 @@
       <c r="F22" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
       <c r="J22" s="34" t="s">
         <v>59</v>
       </c>
@@ -1821,10 +1827,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="43"/>
+      <c r="D24" s="46"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1836,10 +1842,10 @@
       <c r="D25" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="44" t="s">
+      <c r="E25" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="45"/>
+      <c r="F25" s="43"/>
       <c r="G25" s="31" t="s">
         <v>59</v>
       </c>
@@ -1848,10 +1854,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="43" t="s">
+      <c r="I26" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="J26" s="43"/>
+      <c r="J26" s="46"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1866,24 +1872,24 @@
       <c r="J27" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="K27" s="44" t="s">
+      <c r="K27" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="L27" s="45"/>
-      <c r="M27" s="44" t="s">
+      <c r="L27" s="43"/>
+      <c r="M27" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="N27" s="51"/>
-      <c r="O27" s="42" t="s">
+      <c r="N27" s="44"/>
+      <c r="O27" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="P27" s="42"/>
+      <c r="P27" s="40"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="43" t="s">
+      <c r="C29" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="46"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1898,14 +1904,14 @@
       <c r="E30" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="F30" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="H30" s="42" t="s">
+      <c r="G30" s="43"/>
+      <c r="H30" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="42"/>
+      <c r="I30" s="40"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1929,10 +1935,10 @@
       <c r="J32" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="K32" s="44" t="s">
+      <c r="K32" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="L32" s="45"/>
+      <c r="L32" s="43"/>
       <c r="M32" s="33" t="s">
         <v>59</v>
       </c>
@@ -2086,10 +2092,10 @@
       <c r="B58" s="20">
         <v>81</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C58" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="41"/>
+      <c r="D58" s="51"/>
       <c r="E58" s="1" t="s">
         <v>2</v>
       </c>
@@ -2423,10 +2429,10 @@
       <c r="B106" s="20">
         <v>87</v>
       </c>
-      <c r="C106" s="40" t="s">
+      <c r="C106" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="D106" s="40"/>
+      <c r="D106" s="50"/>
       <c r="E106" s="38" t="s">
         <v>91</v>
       </c>
@@ -2446,6 +2452,9 @@
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B109" t="s">
+        <v>125</v>
+      </c>
       <c r="G109" s="10" t="s">
         <v>6</v>
       </c>
@@ -2453,7 +2462,21 @@
         <v>106</v>
       </c>
     </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="20">
+        <v>89</v>
+      </c>
+      <c r="C110" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
+        <v>126</v>
+      </c>
       <c r="H111" t="s">
         <v>108</v>
       </c>
@@ -2475,15 +2498,12 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I112:J112"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="I104:J104"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2495,12 +2515,15 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="I104:J104"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="I112:J112"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change version info and store it on node structure
Now it is added to node info in API
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCB5F36-E4E5-41DD-AB3D-3FDEB8BA690A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F5C1A0-C1FF-46FF-82A2-7720BE3A2610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5070" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>Message type. Unencrypted</t>
   </si>
   <si>
-    <t>ASCII encoded version (f.i. "0.2.0")</t>
-  </si>
-  <si>
     <t>Sleep time (32 bits integer)</t>
   </si>
   <si>
@@ -403,6 +400,9 @@
   </si>
   <si>
     <t>Sent on intentional restart</t>
+  </si>
+  <si>
+    <t>Version (3 bytes)</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:U112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1539,7 +1539,7 @@
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
       <c r="C4" s="45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -1570,22 +1570,22 @@
         <v>0</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>24</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="40"/>
       <c r="J6" s="1" t="s">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="K6" s="10"/>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
@@ -1605,7 +1605,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>6</v>
@@ -1614,10 +1614,10 @@
         <v>1</v>
       </c>
       <c r="I8" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K8" s="36" t="s">
         <v>5</v>
@@ -1626,11 +1626,11 @@
         <v>17</v>
       </c>
       <c r="M8" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N8" s="40"/>
       <c r="O8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
@@ -1651,7 +1651,7 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
@@ -1659,7 +1659,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>16</v>
@@ -1668,29 +1668,29 @@
         <v>5</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" s="43"/>
       <c r="K13" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="O13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="I14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
@@ -1698,10 +1698,10 @@
         <v>6</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="35" t="s">
         <v>16</v>
@@ -1710,27 +1710,27 @@
         <v>5</v>
       </c>
       <c r="L15" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O15" s="8"/>
       <c r="P15" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q15" s="40"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2"/>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
@@ -1741,13 +1741,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" s="48"/>
       <c r="H17" s="49"/>
@@ -1766,10 +1766,10 @@
         <v>6</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I20" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" s="35" t="s">
         <v>16</v>
@@ -1778,14 +1778,14 @@
         <v>5</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M20" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N20" s="41"/>
       <c r="O20" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P20" s="40"/>
     </row>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="H21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.2">
@@ -1803,7 +1803,7 @@
         <v>28</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>16</v>
@@ -1812,15 +1812,15 @@
         <v>5</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H22" s="41"/>
       <c r="I22" s="41"/>
       <c r="J22" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>2</v>
@@ -1828,26 +1828,26 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C24" s="46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="46"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" s="43"/>
       <c r="G25" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>2</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I26" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J26" s="46"/>
     </row>
@@ -1864,52 +1864,52 @@
         <v>6</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I27" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K27" s="42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L27" s="43"/>
       <c r="M27" s="42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N27" s="44"/>
       <c r="O27" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P27" s="40"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C29" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D29" s="46"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G30" s="43"/>
       <c r="H30" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I30" s="40"/>
       <c r="J30" s="1" t="s">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="I31" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J31" s="32"/>
     </row>
@@ -1927,29 +1927,29 @@
         <v>6</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I32" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K32" s="42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L32" s="43"/>
       <c r="M32" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="3:21" x14ac:dyDescent="0.2">
       <c r="G33" s="10"/>
       <c r="I33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.2">
@@ -1957,7 +1957,7 @@
     </row>
     <row r="35" spans="3:21" x14ac:dyDescent="0.2">
       <c r="F35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -1966,7 +1966,7 @@
         <v>19</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="3:21" x14ac:dyDescent="0.2">
@@ -1974,12 +1974,12 @@
         <v>18</v>
       </c>
       <c r="F37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="3:21" x14ac:dyDescent="0.2">
@@ -1998,7 +1998,7 @@
         <v>10</v>
       </c>
       <c r="J42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R42" t="s">
         <v>12</v>
@@ -2017,7 +2017,7 @@
       <c r="F43" s="1"/>
       <c r="H43" s="1"/>
       <c r="J43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.2">
@@ -2048,7 +2048,7 @@
       </c>
       <c r="D47" s="4"/>
       <c r="E47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="3:21" x14ac:dyDescent="0.2">
@@ -2071,12 +2071,12 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C53" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G56" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
@@ -2093,7 +2093,7 @@
         <v>81</v>
       </c>
       <c r="C58" s="51" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D58" s="51"/>
       <c r="E58" s="1" t="s">
@@ -2103,7 +2103,7 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
@@ -2119,7 +2119,7 @@
         <v>82</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="22"/>
       <c r="E62" s="1" t="s">
@@ -2128,7 +2128,7 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
@@ -2139,7 +2139,7 @@
         <v>28</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I65" s="22"/>
     </row>
@@ -2148,7 +2148,7 @@
         <v>82</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D66" s="22"/>
       <c r="E66" s="1" t="s">
@@ -2158,7 +2158,7 @@
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E67" s="1"/>
       <c r="G67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
@@ -2172,7 +2172,7 @@
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
@@ -2180,10 +2180,10 @@
         <v>6</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H71" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I71" s="23"/>
       <c r="J71" s="23"/>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E73" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
@@ -2199,33 +2199,33 @@
         <v>6</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F74" s="27"/>
       <c r="G74" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H74" s="29"/>
       <c r="I74" s="28"/>
       <c r="J74" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K74" s="29"/>
       <c r="L74" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M74" s="29"/>
       <c r="N74" s="30"/>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C76" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E76" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>2</v>
@@ -2236,20 +2236,20 @@
         <v>6</v>
       </c>
       <c r="E78" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F78" s="27"/>
       <c r="G78" s="28"/>
       <c r="H78" s="29"/>
       <c r="I78" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J78" s="29"/>
       <c r="K78" s="30"/>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D80" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>0</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D82" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>0</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D84" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>0</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D86" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E86" s="19" t="s">
         <v>0</v>
@@ -2300,7 +2300,7 @@
         <v>26</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H86" s="25"/>
       <c r="I86" s="25"/>
@@ -2310,13 +2310,13 @@
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D88" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>2</v>
@@ -2324,13 +2324,13 @@
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D90" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>2</v>
@@ -2338,18 +2338,18 @@
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G93" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H93" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.2">
@@ -2362,18 +2362,18 @@
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G97" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H97" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.2">
@@ -2381,10 +2381,10 @@
         <v>86</v>
       </c>
       <c r="C98" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D98" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>2</v>
@@ -2392,7 +2392,7 @@
     </row>
     <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.2">
@@ -2400,12 +2400,12 @@
         <v>6</v>
       </c>
       <c r="H101" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H103" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.2">
@@ -2413,16 +2413,16 @@
         <v>6</v>
       </c>
       <c r="H104" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I104" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J104" s="39"/>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.2">
@@ -2430,11 +2430,11 @@
         <v>87</v>
       </c>
       <c r="C106" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D106" s="50"/>
       <c r="E106" s="38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F106" s="39"/>
       <c r="G106" s="1" t="s">
@@ -2443,23 +2443,23 @@
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C107" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
       <c r="H108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G109" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H109" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="110" spans="2:11" x14ac:dyDescent="0.2">
@@ -2475,10 +2475,10 @@
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H111" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.2">
@@ -2486,14 +2486,14 @@
         <v>6</v>
       </c>
       <c r="H112" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I112" s="38" t="s">
         <v>123</v>
-      </c>
-      <c r="I112" s="38" t="s">
-        <v>124</v>
       </c>
       <c r="J112" s="39"/>
       <c r="K112" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Define new homeassistant discovery message
</commit_message>
<xml_diff>
--- a/img/Protocol.xlsx
+++ b/img/Protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gmartin\Documents\Arduino\libraries\EnigmaIOT\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F5C1A0-C1FF-46FF-82A2-7720BE3A2610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07895154-D80A-48AC-BF60-16EB9570A659}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="465" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="128">
   <si>
     <t>FF</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Version (3 bytes)</t>
+  </si>
+  <si>
+    <t>HomeAssistantDiscovery</t>
   </si>
 </sst>
 </file>
@@ -841,7 +844,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
@@ -898,16 +901,31 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -916,14 +934,8 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -934,10 +946,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1513,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:U112"/>
+  <dimension ref="B4:U114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58:D58"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1538,21 +1547,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:17" ht="18" x14ac:dyDescent="0.25">
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="J4" s="45" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="J4" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
@@ -1584,10 +1593,10 @@
       <c r="G6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="40"/>
+      <c r="I6" s="45"/>
       <c r="J6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1625,10 +1634,10 @@
       <c r="L8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="N8" s="40"/>
+      <c r="N8" s="45"/>
       <c r="O8" t="s">
         <v>59</v>
       </c>
@@ -1670,14 +1679,14 @@
       <c r="F13" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42" t="s">
+      <c r="H13" s="49"/>
+      <c r="I13" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="J13" s="43"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="34" t="s">
         <v>58</v>
       </c>
@@ -1719,10 +1728,10 @@
         <v>102</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="P15" s="40" t="s">
+      <c r="P15" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="Q15" s="40"/>
+      <c r="Q15" s="45"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
@@ -1746,11 +1755,11 @@
       <c r="E17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="52"/>
       <c r="I17" s="1" t="s">
         <v>2</v>
       </c>
@@ -1780,14 +1789,14 @@
       <c r="L20" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="M20" s="41" t="s">
+      <c r="M20" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="N20" s="41"/>
-      <c r="O20" s="40" t="s">
+      <c r="N20" s="49"/>
+      <c r="O20" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="P20" s="40"/>
+      <c r="P20" s="45"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
@@ -1814,11 +1823,11 @@
       <c r="F22" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="41" t="s">
+      <c r="G22" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
       <c r="J22" s="34" t="s">
         <v>58</v>
       </c>
@@ -1827,10 +1836,10 @@
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="46"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="9" t="s">
@@ -1842,10 +1851,10 @@
       <c r="D25" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E25" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="43"/>
+      <c r="F25" s="48"/>
       <c r="G25" s="31" t="s">
         <v>58</v>
       </c>
@@ -1854,10 +1863,10 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="I26" s="46" t="s">
+      <c r="I26" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="J26" s="46"/>
+      <c r="J26" s="40"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="G27" s="10" t="s">
@@ -1872,24 +1881,24 @@
       <c r="J27" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="42" t="s">
+      <c r="K27" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="L27" s="43"/>
-      <c r="M27" s="42" t="s">
+      <c r="L27" s="48"/>
+      <c r="M27" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="N27" s="44"/>
-      <c r="O27" s="40" t="s">
+      <c r="N27" s="53"/>
+      <c r="O27" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="P27" s="40"/>
+      <c r="P27" s="45"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="46"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="9" t="s">
@@ -1904,14 +1913,14 @@
       <c r="E30" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="43"/>
-      <c r="H30" s="40" t="s">
+      <c r="G30" s="48"/>
+      <c r="H30" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="I30" s="40"/>
+      <c r="I30" s="45"/>
       <c r="J30" s="1" t="s">
         <v>2</v>
       </c>
@@ -1935,15 +1944,15 @@
       <c r="J32" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="K32" s="42" t="s">
+      <c r="K32" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="L32" s="43"/>
+      <c r="L32" s="48"/>
       <c r="M32" s="33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
       <c r="G33" s="10"/>
       <c r="I33" t="s">
         <v>104</v>
@@ -1952,324 +1961,351 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="F35" t="s">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C34" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="40"/>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" s="49"/>
+      <c r="I35" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="J35" s="48"/>
+      <c r="K35" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="G36" s="10"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
         <v>108</v>
       </c>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
         <v>19</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F38" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
         <v>18</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F39" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I41" s="2" t="s">
+    <row r="43" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="F42" s="1" t="s">
+    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I42" s="34" t="s">
+      <c r="I44" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J44" t="s">
         <v>118</v>
       </c>
-      <c r="R42" t="s">
+      <c r="R44" t="s">
         <v>12</v>
       </c>
-      <c r="S42">
+      <c r="S44">
         <v>6</v>
       </c>
-      <c r="T42">
+      <c r="T44">
         <v>2</v>
       </c>
-      <c r="U42">
+      <c r="U44">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="F43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="J43" t="s">
+    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="F45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="J45" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
+    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
         <v>20</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I46" t="s">
         <v>11</v>
       </c>
-      <c r="S44" t="s">
+      <c r="S46" t="s">
         <v>13</v>
       </c>
-      <c r="T44" t="s">
+      <c r="T46" t="s">
         <v>14</v>
       </c>
-      <c r="U44" t="s">
+      <c r="U46" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="I45" t="s">
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C47" s="4" t="s">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="E47" t="s">
+      <c r="D49" s="4"/>
+      <c r="E49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C48" s="11" t="s">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C50" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C49" s="3" t="s">
+      <c r="D50" s="11"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C50" s="5" t="s">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C52" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="5"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C53" s="12" t="s">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C55" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G56" s="14" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G58" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F57" s="10" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F59" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="G59" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="15"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="20">
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="20">
         <v>81</v>
       </c>
-      <c r="C58" s="51" t="s">
+      <c r="C60" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="51"/>
-      <c r="E58" s="1" t="s">
+      <c r="D60" s="44"/>
+      <c r="E60" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G58" s="16"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G60" t="s">
+      <c r="G60" s="16"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F61" s="10" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F63" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="17" t="s">
+      <c r="G63" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="19">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="19">
         <v>82</v>
       </c>
-      <c r="C62" s="21" t="s">
+      <c r="C64" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="1" t="s">
+      <c r="D64" s="22"/>
+      <c r="E64" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G64" t="s">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F65" s="10" t="s">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F67" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="18" t="s">
+      <c r="G67" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H65" s="21" t="s">
+      <c r="H67" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I65" s="22"/>
-    </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B66" s="19">
+      <c r="I67" s="22"/>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B68" s="19">
         <v>82</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C68" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="22"/>
-      <c r="E66" s="1" t="s">
+      <c r="D68" s="22"/>
+      <c r="E68" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E67" s="1"/>
-      <c r="G67" t="s">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E69" s="1"/>
+      <c r="G69" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E68" s="1"/>
-      <c r="F68" s="10" t="s">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E70" s="1"/>
+      <c r="F70" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G68" s="17" t="s">
+      <c r="G70" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="G70" t="s">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="F71" s="10" t="s">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="F73" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G71" s="19" t="s">
+      <c r="G73" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H71" s="21" t="s">
+      <c r="H73" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="I71" s="23"/>
-      <c r="J71" s="23"/>
-      <c r="K71" s="22"/>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="E73" s="12" t="s">
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="22"/>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="E75" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D74" s="10" t="s">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D76" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E74" s="26" t="s">
+      <c r="E76" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F74" s="27"/>
-      <c r="G74" s="28" t="s">
+      <c r="F76" s="27"/>
+      <c r="G76" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="H74" s="29"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28" t="s">
+      <c r="H76" s="29"/>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="K74" s="29"/>
-      <c r="L74" s="28" t="s">
+      <c r="K76" s="29"/>
+      <c r="L76" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="M74" s="29"/>
-      <c r="N74" s="30"/>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C76" s="13" t="s">
+      <c r="M76" s="29"/>
+      <c r="N76" s="30"/>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C78" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D78" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E76" s="24" t="s">
+      <c r="E78" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F78" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D78" s="10" t="s">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D80" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E78" s="26" t="s">
+      <c r="E80" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F78" s="27"/>
-      <c r="G78" s="28"/>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29" t="s">
+      <c r="F80" s="27"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="J78" s="29"/>
-      <c r="K78" s="30"/>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D80" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="J80" s="29"/>
+      <c r="K80" s="30"/>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D82" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>0</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>2</v>
@@ -2277,13 +2313,13 @@
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D84" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>0</v>
       </c>
       <c r="F84" s="25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G84" s="1" t="s">
         <v>2</v>
@@ -2291,219 +2327,238 @@
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D86" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E86" s="19" t="s">
         <v>0</v>
       </c>
       <c r="F86" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="G86" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="H86" s="25"/>
-      <c r="I86" s="25"/>
-      <c r="J86" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D88" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E88" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E88" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F88" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G88" s="1" t="s">
+      <c r="F88" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D90" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>0</v>
       </c>
       <c r="F90" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H92" t="s">
+      <c r="D92" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="95" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B95" t="s">
         <v>74</v>
       </c>
-      <c r="G93" s="10" t="s">
+      <c r="G95" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H93" s="17" t="s">
+      <c r="H95" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B94" s="20">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B96" s="20">
         <v>85</v>
       </c>
-      <c r="F94" s="1" t="s">
+      <c r="F96" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H96" t="s">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B97" t="s">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B99" t="s">
         <v>71</v>
       </c>
-      <c r="G97" s="10" t="s">
+      <c r="G99" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H97" s="17" t="s">
+      <c r="H99" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="20">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B100" s="20">
         <v>86</v>
       </c>
-      <c r="C98" s="24" t="s">
+      <c r="C100" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D98" s="24" t="s">
+      <c r="D100" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="F100" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H100" t="s">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G101" s="10" t="s">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G103" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H101" s="17" t="s">
+      <c r="H103" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H103" t="s">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G104" s="10" t="s">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="G106" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H104" s="17" t="s">
+      <c r="H106" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="I104" s="38" t="s">
+      <c r="I106" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="J104" s="39"/>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B105" t="s">
+      <c r="J106" s="42"/>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B107" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B106" s="20">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B108" s="20">
         <v>87</v>
       </c>
-      <c r="C106" s="50" t="s">
+      <c r="C108" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D106" s="50"/>
-      <c r="E106" s="38" t="s">
+      <c r="D108" s="43"/>
+      <c r="E108" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="F106" s="39"/>
-      <c r="G106" s="1" t="s">
+      <c r="F108" s="42"/>
+      <c r="G108" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C107" t="s">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C109" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="H108" t="s">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B109" t="s">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B111" t="s">
         <v>124</v>
       </c>
-      <c r="G109" s="10" t="s">
+      <c r="G111" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H109" s="17" t="s">
+      <c r="H111" s="17" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="20">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B112" s="20">
         <v>89</v>
       </c>
-      <c r="C110" s="24" t="s">
+      <c r="C112" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F110" s="1" t="s">
+      <c r="F112" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" t="s">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B113" t="s">
         <v>125</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H113" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G112" s="10" t="s">
+    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G114" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H112" s="17" t="s">
+      <c r="H114" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="I112" s="38" t="s">
+      <c r="I114" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="J112" s="39"/>
-      <c r="K112" t="s">
+      <c r="J114" s="42"/>
+      <c r="K114" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="I104:J104"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="H30:I30"/>
+  <mergeCells count="29">
+    <mergeCell ref="I114:J114"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
     <mergeCell ref="J4:O4"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C24:D24"/>
@@ -2515,20 +2570,18 @@
     <mergeCell ref="M20:N20"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I112:J112"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="I106:J106"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B21:B22 I77 I79 F80:F90 E76 B25 H97 H93 B30 H32 H101 H104 H27 G57:G68 H109 B13" numberStoredAsText="1"/>
+    <ignoredError sqref="B21:B22 I79 I81 F82:F92 E78 B25 H99 H95 B30 H32 H103 H106 H27 G59:G70 H111 B13 B35" numberStoredAsText="1"/>
     <ignoredError sqref="H20" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>

</xml_diff>